<commit_message>
shopping cart documents initial commit
</commit_message>
<xml_diff>
--- a/Docs/ShoppingCart WBF.xlsx
+++ b/Docs/ShoppingCart WBF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Effort Summary" sheetId="3" r:id="rId1"/>
@@ -815,38 +815,11 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -867,6 +840,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1562,21 +1562,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="BO129" sqref="BO129:BQ129"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="12" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" customWidth="1"/>
     <col min="13" max="21" width="3.85546875" customWidth="1"/>
     <col min="22" max="22" width="4" customWidth="1"/>
@@ -1587,532 +1589,532 @@
       <c r="A1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="61"/>
+      <c r="C1" s="52"/>
       <c r="D1" s="20"/>
       <c r="E1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="20"/>
       <c r="E2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="53">
         <f>SUM(G9:G137)</f>
         <v>472</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:77" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M4" s="50">
+      <c r="M4" s="49">
         <v>43983</v>
       </c>
-      <c r="N4" s="50">
+      <c r="N4" s="49">
         <v>43984</v>
       </c>
-      <c r="O4" s="50">
+      <c r="O4" s="49">
         <v>43985</v>
       </c>
-      <c r="P4" s="50">
+      <c r="P4" s="49">
         <v>43986</v>
       </c>
-      <c r="Q4" s="50">
+      <c r="Q4" s="49">
         <v>43987</v>
       </c>
-      <c r="R4" s="50">
+      <c r="R4" s="49">
         <v>43990</v>
       </c>
-      <c r="S4" s="50">
+      <c r="S4" s="49">
         <v>43991</v>
       </c>
-      <c r="T4" s="50">
+      <c r="T4" s="49">
         <v>43992</v>
       </c>
-      <c r="U4" s="50">
+      <c r="U4" s="49">
         <v>43993</v>
       </c>
-      <c r="V4" s="50">
+      <c r="V4" s="49">
         <v>43994</v>
       </c>
-      <c r="W4" s="50">
+      <c r="W4" s="49">
         <v>43997</v>
       </c>
-      <c r="X4" s="50">
+      <c r="X4" s="49">
         <v>43998</v>
       </c>
-      <c r="Y4" s="50">
+      <c r="Y4" s="49">
         <v>43999</v>
       </c>
-      <c r="Z4" s="50">
+      <c r="Z4" s="49">
         <v>44000</v>
       </c>
-      <c r="AA4" s="50">
+      <c r="AA4" s="49">
         <v>44001</v>
       </c>
-      <c r="AB4" s="50">
+      <c r="AB4" s="49">
         <v>44004</v>
       </c>
-      <c r="AC4" s="50">
+      <c r="AC4" s="49">
         <v>44005</v>
       </c>
-      <c r="AD4" s="50">
+      <c r="AD4" s="49">
         <v>44006</v>
       </c>
-      <c r="AE4" s="50">
+      <c r="AE4" s="49">
         <v>44007</v>
       </c>
-      <c r="AF4" s="50">
+      <c r="AF4" s="49">
         <v>44008</v>
       </c>
-      <c r="AG4" s="50">
+      <c r="AG4" s="49">
         <v>44011</v>
       </c>
-      <c r="AH4" s="50">
+      <c r="AH4" s="49">
         <v>44012</v>
       </c>
-      <c r="AI4" s="50">
+      <c r="AI4" s="49">
         <v>44013</v>
       </c>
-      <c r="AJ4" s="50">
+      <c r="AJ4" s="49">
         <v>44014</v>
       </c>
-      <c r="AK4" s="50">
+      <c r="AK4" s="49">
         <v>44015</v>
       </c>
-      <c r="AL4" s="50">
+      <c r="AL4" s="49">
         <v>44018</v>
       </c>
-      <c r="AM4" s="50">
+      <c r="AM4" s="49">
         <v>44019</v>
       </c>
-      <c r="AN4" s="50">
+      <c r="AN4" s="49">
         <v>44020</v>
       </c>
-      <c r="AO4" s="50">
+      <c r="AO4" s="49">
         <v>44021</v>
       </c>
-      <c r="AP4" s="50">
+      <c r="AP4" s="49">
         <v>44022</v>
       </c>
-      <c r="AQ4" s="50">
+      <c r="AQ4" s="49">
         <v>44025</v>
       </c>
-      <c r="AR4" s="50">
+      <c r="AR4" s="49">
         <v>44026</v>
       </c>
-      <c r="AS4" s="50">
+      <c r="AS4" s="49">
         <v>44027</v>
       </c>
-      <c r="AT4" s="50">
+      <c r="AT4" s="49">
         <v>44028</v>
       </c>
-      <c r="AU4" s="50">
+      <c r="AU4" s="49">
         <v>44029</v>
       </c>
-      <c r="AV4" s="50">
+      <c r="AV4" s="49">
         <v>44032</v>
       </c>
-      <c r="AW4" s="50">
+      <c r="AW4" s="49">
         <v>44033</v>
       </c>
-      <c r="AX4" s="50">
+      <c r="AX4" s="49">
         <v>44034</v>
       </c>
-      <c r="AY4" s="50">
+      <c r="AY4" s="49">
         <v>44035</v>
       </c>
-      <c r="AZ4" s="50">
+      <c r="AZ4" s="49">
         <v>44036</v>
       </c>
-      <c r="BA4" s="50">
+      <c r="BA4" s="49">
         <v>44039</v>
       </c>
-      <c r="BB4" s="50">
+      <c r="BB4" s="49">
         <v>44040</v>
       </c>
-      <c r="BC4" s="50">
+      <c r="BC4" s="49">
         <v>44041</v>
       </c>
-      <c r="BD4" s="50">
+      <c r="BD4" s="49">
         <v>44042</v>
       </c>
-      <c r="BE4" s="50">
+      <c r="BE4" s="49">
         <v>44043</v>
       </c>
-      <c r="BF4" s="50">
+      <c r="BF4" s="49">
         <v>44046</v>
       </c>
-      <c r="BG4" s="50">
+      <c r="BG4" s="49">
         <v>44047</v>
       </c>
-      <c r="BH4" s="50">
+      <c r="BH4" s="49">
         <v>44048</v>
       </c>
-      <c r="BI4" s="50">
+      <c r="BI4" s="49">
         <v>44049</v>
       </c>
-      <c r="BJ4" s="50">
+      <c r="BJ4" s="49">
         <v>44050</v>
       </c>
-      <c r="BK4" s="50">
+      <c r="BK4" s="49">
         <v>44053</v>
       </c>
-      <c r="BL4" s="50">
+      <c r="BL4" s="49">
         <v>44054</v>
       </c>
-      <c r="BM4" s="50">
+      <c r="BM4" s="49">
         <v>44055</v>
       </c>
-      <c r="BN4" s="50">
+      <c r="BN4" s="49">
         <v>44056</v>
       </c>
-      <c r="BO4" s="50">
+      <c r="BO4" s="49">
         <v>44057</v>
       </c>
-      <c r="BP4" s="50">
+      <c r="BP4" s="49">
         <v>44060</v>
       </c>
-      <c r="BQ4" s="50">
+      <c r="BQ4" s="49">
         <v>44061</v>
       </c>
-      <c r="BR4" s="50">
+      <c r="BR4" s="49">
         <v>44062</v>
       </c>
-      <c r="BS4" s="50">
+      <c r="BS4" s="49">
         <v>44063</v>
       </c>
-      <c r="BT4" s="50">
+      <c r="BT4" s="49">
         <v>44064</v>
       </c>
-      <c r="BU4" s="50">
+      <c r="BU4" s="49">
         <v>44067</v>
       </c>
-      <c r="BV4" s="50">
+      <c r="BV4" s="49">
         <v>44068</v>
       </c>
-      <c r="BW4" s="50">
+      <c r="BW4" s="49">
         <v>44069</v>
       </c>
-      <c r="BX4" s="50">
+      <c r="BX4" s="49">
         <v>44070</v>
       </c>
-      <c r="BY4" s="50">
+      <c r="BY4" s="49">
         <v>44071</v>
       </c>
     </row>
     <row r="5" spans="1:77" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="50"/>
-      <c r="AG5" s="50"/>
-      <c r="AH5" s="50"/>
-      <c r="AI5" s="50"/>
-      <c r="AJ5" s="50"/>
-      <c r="AK5" s="50"/>
-      <c r="AL5" s="50"/>
-      <c r="AM5" s="50"/>
-      <c r="AN5" s="50"/>
-      <c r="AO5" s="50"/>
-      <c r="AP5" s="50"/>
-      <c r="AQ5" s="50"/>
-      <c r="AR5" s="50"/>
-      <c r="AS5" s="50"/>
-      <c r="AT5" s="50"/>
-      <c r="AU5" s="50"/>
-      <c r="AV5" s="50"/>
-      <c r="AW5" s="50"/>
-      <c r="AX5" s="50"/>
-      <c r="AY5" s="50"/>
-      <c r="AZ5" s="50"/>
-      <c r="BA5" s="50"/>
-      <c r="BB5" s="50"/>
-      <c r="BC5" s="50"/>
-      <c r="BD5" s="50"/>
-      <c r="BE5" s="50"/>
-      <c r="BF5" s="50"/>
-      <c r="BG5" s="50"/>
-      <c r="BH5" s="50"/>
-      <c r="BI5" s="50"/>
-      <c r="BJ5" s="50"/>
-      <c r="BK5" s="50"/>
-      <c r="BL5" s="50"/>
-      <c r="BM5" s="50"/>
-      <c r="BN5" s="50"/>
-      <c r="BO5" s="50"/>
-      <c r="BP5" s="50"/>
-      <c r="BQ5" s="50"/>
-      <c r="BR5" s="50"/>
-      <c r="BS5" s="50"/>
-      <c r="BT5" s="50"/>
-      <c r="BU5" s="50"/>
-      <c r="BV5" s="50"/>
-      <c r="BW5" s="50"/>
-      <c r="BX5" s="50"/>
-      <c r="BY5" s="50"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
+      <c r="AQ5" s="49"/>
+      <c r="AR5" s="49"/>
+      <c r="AS5" s="49"/>
+      <c r="AT5" s="49"/>
+      <c r="AU5" s="49"/>
+      <c r="AV5" s="49"/>
+      <c r="AW5" s="49"/>
+      <c r="AX5" s="49"/>
+      <c r="AY5" s="49"/>
+      <c r="AZ5" s="49"/>
+      <c r="BA5" s="49"/>
+      <c r="BB5" s="49"/>
+      <c r="BC5" s="49"/>
+      <c r="BD5" s="49"/>
+      <c r="BE5" s="49"/>
+      <c r="BF5" s="49"/>
+      <c r="BG5" s="49"/>
+      <c r="BH5" s="49"/>
+      <c r="BI5" s="49"/>
+      <c r="BJ5" s="49"/>
+      <c r="BK5" s="49"/>
+      <c r="BL5" s="49"/>
+      <c r="BM5" s="49"/>
+      <c r="BN5" s="49"/>
+      <c r="BO5" s="49"/>
+      <c r="BP5" s="49"/>
+      <c r="BQ5" s="49"/>
+      <c r="BR5" s="49"/>
+      <c r="BS5" s="49"/>
+      <c r="BT5" s="49"/>
+      <c r="BU5" s="49"/>
+      <c r="BV5" s="49"/>
+      <c r="BW5" s="49"/>
+      <c r="BX5" s="49"/>
+      <c r="BY5" s="49"/>
     </row>
     <row r="6" spans="1:77" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="51"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="51"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="51"/>
-      <c r="Y6" s="51"/>
-      <c r="Z6" s="51"/>
-      <c r="AA6" s="51"/>
-      <c r="AB6" s="51"/>
-      <c r="AC6" s="51"/>
-      <c r="AD6" s="51"/>
-      <c r="AE6" s="51"/>
-      <c r="AF6" s="51"/>
-      <c r="AG6" s="51"/>
-      <c r="AH6" s="51"/>
-      <c r="AI6" s="51"/>
-      <c r="AJ6" s="51"/>
-      <c r="AK6" s="51"/>
-      <c r="AL6" s="51"/>
-      <c r="AM6" s="51"/>
-      <c r="AN6" s="51"/>
-      <c r="AO6" s="51"/>
-      <c r="AP6" s="51"/>
-      <c r="AQ6" s="51"/>
-      <c r="AR6" s="51"/>
-      <c r="AS6" s="51"/>
-      <c r="AT6" s="51"/>
-      <c r="AU6" s="51"/>
-      <c r="AV6" s="51"/>
-      <c r="AW6" s="51"/>
-      <c r="AX6" s="51"/>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="51"/>
-      <c r="BA6" s="51"/>
-      <c r="BB6" s="51"/>
-      <c r="BC6" s="51"/>
-      <c r="BD6" s="51"/>
-      <c r="BE6" s="51"/>
-      <c r="BF6" s="51"/>
-      <c r="BG6" s="51"/>
-      <c r="BH6" s="51"/>
-      <c r="BI6" s="51"/>
-      <c r="BJ6" s="51"/>
-      <c r="BK6" s="51"/>
-      <c r="BL6" s="51"/>
-      <c r="BM6" s="51"/>
-      <c r="BN6" s="51"/>
-      <c r="BO6" s="51"/>
-      <c r="BP6" s="51"/>
-      <c r="BQ6" s="51"/>
-      <c r="BR6" s="51"/>
-      <c r="BS6" s="51"/>
-      <c r="BT6" s="51"/>
-      <c r="BU6" s="51"/>
-      <c r="BV6" s="51"/>
-      <c r="BW6" s="51"/>
-      <c r="BX6" s="51"/>
-      <c r="BY6" s="51"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="R6" s="50"/>
+      <c r="S6" s="50"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="50"/>
+      <c r="X6" s="50"/>
+      <c r="Y6" s="50"/>
+      <c r="Z6" s="50"/>
+      <c r="AA6" s="50"/>
+      <c r="AB6" s="50"/>
+      <c r="AC6" s="50"/>
+      <c r="AD6" s="50"/>
+      <c r="AE6" s="50"/>
+      <c r="AF6" s="50"/>
+      <c r="AG6" s="50"/>
+      <c r="AH6" s="50"/>
+      <c r="AI6" s="50"/>
+      <c r="AJ6" s="50"/>
+      <c r="AK6" s="50"/>
+      <c r="AL6" s="50"/>
+      <c r="AM6" s="50"/>
+      <c r="AN6" s="50"/>
+      <c r="AO6" s="50"/>
+      <c r="AP6" s="50"/>
+      <c r="AQ6" s="50"/>
+      <c r="AR6" s="50"/>
+      <c r="AS6" s="50"/>
+      <c r="AT6" s="50"/>
+      <c r="AU6" s="50"/>
+      <c r="AV6" s="50"/>
+      <c r="AW6" s="50"/>
+      <c r="AX6" s="50"/>
+      <c r="AY6" s="50"/>
+      <c r="AZ6" s="50"/>
+      <c r="BA6" s="50"/>
+      <c r="BB6" s="50"/>
+      <c r="BC6" s="50"/>
+      <c r="BD6" s="50"/>
+      <c r="BE6" s="50"/>
+      <c r="BF6" s="50"/>
+      <c r="BG6" s="50"/>
+      <c r="BH6" s="50"/>
+      <c r="BI6" s="50"/>
+      <c r="BJ6" s="50"/>
+      <c r="BK6" s="50"/>
+      <c r="BL6" s="50"/>
+      <c r="BM6" s="50"/>
+      <c r="BN6" s="50"/>
+      <c r="BO6" s="50"/>
+      <c r="BP6" s="50"/>
+      <c r="BQ6" s="50"/>
+      <c r="BR6" s="50"/>
+      <c r="BS6" s="50"/>
+      <c r="BT6" s="50"/>
+      <c r="BU6" s="50"/>
+      <c r="BV6" s="50"/>
+      <c r="BW6" s="50"/>
+      <c r="BX6" s="50"/>
+      <c r="BY6" s="50"/>
     </row>
     <row r="7" spans="1:77" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52" t="s">
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="52" t="s">
+      <c r="G7" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="52" t="s">
+      <c r="H7" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="52" t="s">
+      <c r="I7" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="52" t="s">
+      <c r="J7" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="52" t="s">
+      <c r="K7" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="52" t="s">
+      <c r="L7" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="57" t="s">
+      <c r="M7" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="57" t="s">
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="57" t="s">
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="67"/>
+      <c r="W7" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="57" t="s">
+      <c r="X7" s="66"/>
+      <c r="Y7" s="66"/>
+      <c r="Z7" s="66"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="59"/>
-      <c r="AG7" s="49" t="s">
+      <c r="AC7" s="66"/>
+      <c r="AD7" s="66"/>
+      <c r="AE7" s="66"/>
+      <c r="AF7" s="67"/>
+      <c r="AG7" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="AH7" s="49"/>
-      <c r="AI7" s="49"/>
-      <c r="AJ7" s="49"/>
-      <c r="AK7" s="49"/>
-      <c r="AL7" s="49" t="s">
+      <c r="AH7" s="61"/>
+      <c r="AI7" s="61"/>
+      <c r="AJ7" s="61"/>
+      <c r="AK7" s="61"/>
+      <c r="AL7" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="AM7" s="49"/>
-      <c r="AN7" s="49"/>
-      <c r="AO7" s="49"/>
-      <c r="AP7" s="49"/>
-      <c r="AQ7" s="49" t="s">
+      <c r="AM7" s="61"/>
+      <c r="AN7" s="61"/>
+      <c r="AO7" s="61"/>
+      <c r="AP7" s="61"/>
+      <c r="AQ7" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="AR7" s="49"/>
-      <c r="AS7" s="49"/>
-      <c r="AT7" s="49"/>
-      <c r="AU7" s="49"/>
-      <c r="AV7" s="49" t="s">
+      <c r="AR7" s="61"/>
+      <c r="AS7" s="61"/>
+      <c r="AT7" s="61"/>
+      <c r="AU7" s="61"/>
+      <c r="AV7" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="AW7" s="49"/>
-      <c r="AX7" s="49"/>
-      <c r="AY7" s="49"/>
-      <c r="AZ7" s="49"/>
-      <c r="BA7" s="54" t="s">
+      <c r="AW7" s="61"/>
+      <c r="AX7" s="61"/>
+      <c r="AY7" s="61"/>
+      <c r="AZ7" s="61"/>
+      <c r="BA7" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="BB7" s="55"/>
-      <c r="BC7" s="55"/>
-      <c r="BD7" s="55"/>
-      <c r="BE7" s="56"/>
-      <c r="BF7" s="49" t="s">
+      <c r="BB7" s="63"/>
+      <c r="BC7" s="63"/>
+      <c r="BD7" s="63"/>
+      <c r="BE7" s="64"/>
+      <c r="BF7" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="BG7" s="49"/>
-      <c r="BH7" s="49"/>
-      <c r="BI7" s="49"/>
-      <c r="BJ7" s="49"/>
-      <c r="BK7" s="49" t="s">
+      <c r="BG7" s="61"/>
+      <c r="BH7" s="61"/>
+      <c r="BI7" s="61"/>
+      <c r="BJ7" s="61"/>
+      <c r="BK7" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="BL7" s="49"/>
-      <c r="BM7" s="49"/>
-      <c r="BN7" s="49"/>
-      <c r="BO7" s="49"/>
-      <c r="BP7" s="49" t="s">
+      <c r="BL7" s="61"/>
+      <c r="BM7" s="61"/>
+      <c r="BN7" s="61"/>
+      <c r="BO7" s="61"/>
+      <c r="BP7" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="BQ7" s="49"/>
-      <c r="BR7" s="49"/>
-      <c r="BS7" s="49"/>
-      <c r="BT7" s="49"/>
-      <c r="BU7" s="49" t="s">
+      <c r="BQ7" s="61"/>
+      <c r="BR7" s="61"/>
+      <c r="BS7" s="61"/>
+      <c r="BT7" s="61"/>
+      <c r="BU7" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="BV7" s="49"/>
-      <c r="BW7" s="49"/>
-      <c r="BX7" s="49"/>
-      <c r="BY7" s="49"/>
+      <c r="BV7" s="61"/>
+      <c r="BW7" s="61"/>
+      <c r="BX7" s="61"/>
+      <c r="BY7" s="61"/>
     </row>
     <row r="8" spans="1:77" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
       <c r="M8" s="24" t="s">
         <v>75</v>
       </c>
@@ -15558,20 +15560,20 @@
       <c r="BY137" s="33"/>
     </row>
     <row r="138" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A138" s="64" t="s">
+      <c r="A138" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B138" s="65"/>
-      <c r="C138" s="65"/>
-      <c r="D138" s="65"/>
-      <c r="E138" s="65"/>
-      <c r="F138" s="65"/>
-      <c r="G138" s="65"/>
-      <c r="H138" s="65"/>
-      <c r="I138" s="65"/>
-      <c r="J138" s="65"/>
-      <c r="K138" s="65"/>
-      <c r="L138" s="66"/>
+      <c r="B138" s="56"/>
+      <c r="C138" s="56"/>
+      <c r="D138" s="56"/>
+      <c r="E138" s="56"/>
+      <c r="F138" s="56"/>
+      <c r="G138" s="56"/>
+      <c r="H138" s="56"/>
+      <c r="I138" s="56"/>
+      <c r="J138" s="56"/>
+      <c r="K138" s="56"/>
+      <c r="L138" s="57"/>
       <c r="M138" s="37">
         <f>SUM(M10:M135)</f>
         <v>0</v>
@@ -15838,55 +15840,38 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="BG4:BG6"/>
-    <mergeCell ref="BH4:BH6"/>
-    <mergeCell ref="BI4:BI6"/>
-    <mergeCell ref="BJ4:BJ6"/>
-    <mergeCell ref="BB4:BB6"/>
-    <mergeCell ref="BC4:BC6"/>
-    <mergeCell ref="BD4:BD6"/>
-    <mergeCell ref="BE4:BE6"/>
-    <mergeCell ref="BF4:BF6"/>
-    <mergeCell ref="AW4:AW6"/>
-    <mergeCell ref="AX4:AX6"/>
-    <mergeCell ref="AY4:AY6"/>
-    <mergeCell ref="AZ4:AZ6"/>
-    <mergeCell ref="BA4:BA6"/>
-    <mergeCell ref="AR4:AR6"/>
-    <mergeCell ref="AS4:AS6"/>
-    <mergeCell ref="AT4:AT6"/>
-    <mergeCell ref="AU4:AU6"/>
-    <mergeCell ref="AV4:AV6"/>
-    <mergeCell ref="AM4:AM6"/>
-    <mergeCell ref="AN4:AN6"/>
-    <mergeCell ref="AO4:AO6"/>
-    <mergeCell ref="AP4:AP6"/>
-    <mergeCell ref="AQ4:AQ6"/>
-    <mergeCell ref="AH4:AH6"/>
-    <mergeCell ref="AI4:AI6"/>
-    <mergeCell ref="AJ4:AJ6"/>
-    <mergeCell ref="AK4:AK6"/>
-    <mergeCell ref="AL4:AL6"/>
-    <mergeCell ref="AC4:AC6"/>
-    <mergeCell ref="AD4:AD6"/>
-    <mergeCell ref="AE4:AE6"/>
-    <mergeCell ref="AF4:AF6"/>
-    <mergeCell ref="AG4:AG6"/>
-    <mergeCell ref="X4:X6"/>
-    <mergeCell ref="Y4:Y6"/>
-    <mergeCell ref="Z4:Z6"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="AB4:AB6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="U4:U6"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="BK7:BO7"/>
+    <mergeCell ref="BP7:BT7"/>
+    <mergeCell ref="BU7:BY7"/>
+    <mergeCell ref="BU4:BU6"/>
+    <mergeCell ref="BV4:BV6"/>
+    <mergeCell ref="BW4:BW6"/>
+    <mergeCell ref="BX4:BX6"/>
+    <mergeCell ref="BY4:BY6"/>
+    <mergeCell ref="BP4:BP6"/>
+    <mergeCell ref="BQ4:BQ6"/>
+    <mergeCell ref="BR4:BR6"/>
+    <mergeCell ref="BS4:BS6"/>
+    <mergeCell ref="BT4:BT6"/>
+    <mergeCell ref="BK4:BK6"/>
+    <mergeCell ref="BL4:BL6"/>
+    <mergeCell ref="BM4:BM6"/>
+    <mergeCell ref="BN4:BN6"/>
+    <mergeCell ref="BO4:BO6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="AL7:AP7"/>
+    <mergeCell ref="AQ7:AU7"/>
+    <mergeCell ref="AV7:AZ7"/>
+    <mergeCell ref="BA7:BE7"/>
+    <mergeCell ref="BF7:BJ7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="M4:M6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A138:L138"/>
@@ -15903,38 +15888,55 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="BN4:BN6"/>
-    <mergeCell ref="BO4:BO6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="AL7:AP7"/>
-    <mergeCell ref="AQ7:AU7"/>
-    <mergeCell ref="AV7:AZ7"/>
-    <mergeCell ref="BA7:BE7"/>
-    <mergeCell ref="BF7:BJ7"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AG7:AK7"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="BK7:BO7"/>
-    <mergeCell ref="BP7:BT7"/>
-    <mergeCell ref="BU7:BY7"/>
-    <mergeCell ref="BU4:BU6"/>
-    <mergeCell ref="BV4:BV6"/>
-    <mergeCell ref="BW4:BW6"/>
-    <mergeCell ref="BX4:BX6"/>
-    <mergeCell ref="BY4:BY6"/>
-    <mergeCell ref="BP4:BP6"/>
-    <mergeCell ref="BQ4:BQ6"/>
-    <mergeCell ref="BR4:BR6"/>
-    <mergeCell ref="BS4:BS6"/>
-    <mergeCell ref="BT4:BT6"/>
-    <mergeCell ref="BK4:BK6"/>
-    <mergeCell ref="BL4:BL6"/>
-    <mergeCell ref="BM4:BM6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="U4:U6"/>
+    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="X4:X6"/>
+    <mergeCell ref="Y4:Y6"/>
+    <mergeCell ref="Z4:Z6"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AB4:AB6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AD4:AD6"/>
+    <mergeCell ref="AE4:AE6"/>
+    <mergeCell ref="AF4:AF6"/>
+    <mergeCell ref="AG4:AG6"/>
+    <mergeCell ref="AH4:AH6"/>
+    <mergeCell ref="AI4:AI6"/>
+    <mergeCell ref="AJ4:AJ6"/>
+    <mergeCell ref="AK4:AK6"/>
+    <mergeCell ref="AL4:AL6"/>
+    <mergeCell ref="AM4:AM6"/>
+    <mergeCell ref="AN4:AN6"/>
+    <mergeCell ref="AO4:AO6"/>
+    <mergeCell ref="AP4:AP6"/>
+    <mergeCell ref="AQ4:AQ6"/>
+    <mergeCell ref="AR4:AR6"/>
+    <mergeCell ref="AS4:AS6"/>
+    <mergeCell ref="AT4:AT6"/>
+    <mergeCell ref="AU4:AU6"/>
+    <mergeCell ref="AV4:AV6"/>
+    <mergeCell ref="AW4:AW6"/>
+    <mergeCell ref="AX4:AX6"/>
+    <mergeCell ref="AY4:AY6"/>
+    <mergeCell ref="AZ4:AZ6"/>
+    <mergeCell ref="BA4:BA6"/>
+    <mergeCell ref="BG4:BG6"/>
+    <mergeCell ref="BH4:BH6"/>
+    <mergeCell ref="BI4:BI6"/>
+    <mergeCell ref="BJ4:BJ6"/>
+    <mergeCell ref="BB4:BB6"/>
+    <mergeCell ref="BC4:BC6"/>
+    <mergeCell ref="BD4:BD6"/>
+    <mergeCell ref="BE4:BE6"/>
+    <mergeCell ref="BF4:BF6"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E48 E52 E54:E109 E111:E137">
     <cfRule type="cellIs" dxfId="19" priority="20" stopIfTrue="1" operator="greaterThan">

</xml_diff>

<commit_message>
initial enums and add validation for model
</commit_message>
<xml_diff>
--- a/Docs/ShoppingCart WBF.xlsx
+++ b/Docs/ShoppingCart WBF.xlsx
@@ -823,74 +823,6 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
@@ -931,9 +863,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -946,6 +875,77 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1681,10 +1681,10 @@
   <dimension ref="A1:BY141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="12" ySplit="8" topLeftCell="N123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="8" topLeftCell="AC25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="J127" sqref="J127"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,532 +1707,532 @@
       <c r="A1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="43"/>
+      <c r="C1" s="72"/>
       <c r="D1" s="20"/>
       <c r="E1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="43"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="20"/>
       <c r="E2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="73">
         <f>SUM(G9:G139)</f>
         <v>470</v>
       </c>
-      <c r="C3" s="45"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
     </row>
     <row r="4" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M4" s="40">
+      <c r="M4" s="61">
         <v>43983</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="61">
         <v>43984</v>
       </c>
-      <c r="O4" s="40">
+      <c r="O4" s="61">
         <v>43985</v>
       </c>
-      <c r="P4" s="40">
+      <c r="P4" s="61">
         <v>43986</v>
       </c>
-      <c r="Q4" s="40">
+      <c r="Q4" s="61">
         <v>43987</v>
       </c>
-      <c r="R4" s="40">
+      <c r="R4" s="61">
         <v>43990</v>
       </c>
-      <c r="S4" s="40">
+      <c r="S4" s="61">
         <v>43991</v>
       </c>
-      <c r="T4" s="40">
+      <c r="T4" s="61">
         <v>43992</v>
       </c>
-      <c r="U4" s="40">
+      <c r="U4" s="61">
         <v>43993</v>
       </c>
-      <c r="V4" s="40">
+      <c r="V4" s="61">
         <v>43994</v>
       </c>
-      <c r="W4" s="40">
+      <c r="W4" s="61">
         <v>43997</v>
       </c>
-      <c r="X4" s="40">
+      <c r="X4" s="61">
         <v>43998</v>
       </c>
-      <c r="Y4" s="40">
+      <c r="Y4" s="61">
         <v>43999</v>
       </c>
-      <c r="Z4" s="40">
+      <c r="Z4" s="61">
         <v>44000</v>
       </c>
-      <c r="AA4" s="40">
+      <c r="AA4" s="61">
         <v>44001</v>
       </c>
-      <c r="AB4" s="40">
+      <c r="AB4" s="61">
         <v>44004</v>
       </c>
-      <c r="AC4" s="40">
+      <c r="AC4" s="61">
         <v>44005</v>
       </c>
-      <c r="AD4" s="40">
+      <c r="AD4" s="61">
         <v>44006</v>
       </c>
-      <c r="AE4" s="40">
+      <c r="AE4" s="61">
         <v>44007</v>
       </c>
-      <c r="AF4" s="40">
+      <c r="AF4" s="61">
         <v>44008</v>
       </c>
-      <c r="AG4" s="40">
+      <c r="AG4" s="61">
         <v>44011</v>
       </c>
-      <c r="AH4" s="40">
+      <c r="AH4" s="61">
         <v>44012</v>
       </c>
-      <c r="AI4" s="40">
+      <c r="AI4" s="61">
         <v>44013</v>
       </c>
-      <c r="AJ4" s="40">
+      <c r="AJ4" s="61">
         <v>44014</v>
       </c>
-      <c r="AK4" s="40">
+      <c r="AK4" s="61">
         <v>44015</v>
       </c>
-      <c r="AL4" s="40">
+      <c r="AL4" s="61">
         <v>44018</v>
       </c>
-      <c r="AM4" s="40">
+      <c r="AM4" s="61">
         <v>44019</v>
       </c>
-      <c r="AN4" s="40">
+      <c r="AN4" s="61">
         <v>44020</v>
       </c>
-      <c r="AO4" s="40">
+      <c r="AO4" s="61">
         <v>44021</v>
       </c>
-      <c r="AP4" s="40">
+      <c r="AP4" s="61">
         <v>44022</v>
       </c>
-      <c r="AQ4" s="40">
+      <c r="AQ4" s="61">
         <v>44025</v>
       </c>
-      <c r="AR4" s="40">
+      <c r="AR4" s="61">
         <v>44026</v>
       </c>
-      <c r="AS4" s="40">
+      <c r="AS4" s="61">
         <v>44027</v>
       </c>
-      <c r="AT4" s="40">
+      <c r="AT4" s="61">
         <v>44028</v>
       </c>
-      <c r="AU4" s="40">
+      <c r="AU4" s="61">
         <v>44029</v>
       </c>
-      <c r="AV4" s="40">
+      <c r="AV4" s="61">
         <v>44032</v>
       </c>
-      <c r="AW4" s="40">
+      <c r="AW4" s="61">
         <v>44033</v>
       </c>
-      <c r="AX4" s="40">
+      <c r="AX4" s="61">
         <v>44034</v>
       </c>
-      <c r="AY4" s="40">
+      <c r="AY4" s="61">
         <v>44035</v>
       </c>
-      <c r="AZ4" s="40">
+      <c r="AZ4" s="61">
         <v>44036</v>
       </c>
-      <c r="BA4" s="40">
+      <c r="BA4" s="61">
         <v>44039</v>
       </c>
-      <c r="BB4" s="40">
+      <c r="BB4" s="61">
         <v>44040</v>
       </c>
-      <c r="BC4" s="40">
+      <c r="BC4" s="61">
         <v>44041</v>
       </c>
-      <c r="BD4" s="40">
+      <c r="BD4" s="61">
         <v>44042</v>
       </c>
-      <c r="BE4" s="40">
+      <c r="BE4" s="61">
         <v>44043</v>
       </c>
-      <c r="BF4" s="40">
+      <c r="BF4" s="61">
         <v>44046</v>
       </c>
-      <c r="BG4" s="40">
+      <c r="BG4" s="61">
         <v>44047</v>
       </c>
-      <c r="BH4" s="40">
+      <c r="BH4" s="61">
         <v>44048</v>
       </c>
-      <c r="BI4" s="40">
+      <c r="BI4" s="61">
         <v>44049</v>
       </c>
-      <c r="BJ4" s="40">
+      <c r="BJ4" s="61">
         <v>44050</v>
       </c>
-      <c r="BK4" s="40">
+      <c r="BK4" s="61">
         <v>44053</v>
       </c>
-      <c r="BL4" s="40">
+      <c r="BL4" s="61">
         <v>44054</v>
       </c>
-      <c r="BM4" s="40">
+      <c r="BM4" s="61">
         <v>44055</v>
       </c>
-      <c r="BN4" s="40">
+      <c r="BN4" s="61">
         <v>44056</v>
       </c>
-      <c r="BO4" s="40">
+      <c r="BO4" s="61">
         <v>44057</v>
       </c>
-      <c r="BP4" s="40">
+      <c r="BP4" s="61">
         <v>44060</v>
       </c>
-      <c r="BQ4" s="40">
+      <c r="BQ4" s="61">
         <v>44061</v>
       </c>
-      <c r="BR4" s="40">
+      <c r="BR4" s="61">
         <v>44062</v>
       </c>
-      <c r="BS4" s="40">
+      <c r="BS4" s="61">
         <v>44063</v>
       </c>
-      <c r="BT4" s="40">
+      <c r="BT4" s="61">
         <v>44064</v>
       </c>
-      <c r="BU4" s="40">
+      <c r="BU4" s="61">
         <v>44067</v>
       </c>
-      <c r="BV4" s="40">
+      <c r="BV4" s="61">
         <v>44068</v>
       </c>
-      <c r="BW4" s="40">
+      <c r="BW4" s="61">
         <v>44069</v>
       </c>
-      <c r="BX4" s="40">
+      <c r="BX4" s="61">
         <v>44070</v>
       </c>
-      <c r="BY4" s="40">
+      <c r="BY4" s="61">
         <v>44071</v>
       </c>
     </row>
     <row r="5" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="40"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="40"/>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="40"/>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="40"/>
-      <c r="AE5" s="40"/>
-      <c r="AF5" s="40"/>
-      <c r="AG5" s="40"/>
-      <c r="AH5" s="40"/>
-      <c r="AI5" s="40"/>
-      <c r="AJ5" s="40"/>
-      <c r="AK5" s="40"/>
-      <c r="AL5" s="40"/>
-      <c r="AM5" s="40"/>
-      <c r="AN5" s="40"/>
-      <c r="AO5" s="40"/>
-      <c r="AP5" s="40"/>
-      <c r="AQ5" s="40"/>
-      <c r="AR5" s="40"/>
-      <c r="AS5" s="40"/>
-      <c r="AT5" s="40"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="40"/>
-      <c r="AW5" s="40"/>
-      <c r="AX5" s="40"/>
-      <c r="AY5" s="40"/>
-      <c r="AZ5" s="40"/>
-      <c r="BA5" s="40"/>
-      <c r="BB5" s="40"/>
-      <c r="BC5" s="40"/>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="40"/>
-      <c r="BF5" s="40"/>
-      <c r="BG5" s="40"/>
-      <c r="BH5" s="40"/>
-      <c r="BI5" s="40"/>
-      <c r="BJ5" s="40"/>
-      <c r="BK5" s="40"/>
-      <c r="BL5" s="40"/>
-      <c r="BM5" s="40"/>
-      <c r="BN5" s="40"/>
-      <c r="BO5" s="40"/>
-      <c r="BP5" s="40"/>
-      <c r="BQ5" s="40"/>
-      <c r="BR5" s="40"/>
-      <c r="BS5" s="40"/>
-      <c r="BT5" s="40"/>
-      <c r="BU5" s="40"/>
-      <c r="BV5" s="40"/>
-      <c r="BW5" s="40"/>
-      <c r="BX5" s="40"/>
-      <c r="BY5" s="40"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="61"/>
+      <c r="Y5" s="61"/>
+      <c r="Z5" s="61"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="61"/>
+      <c r="AC5" s="61"/>
+      <c r="AD5" s="61"/>
+      <c r="AE5" s="61"/>
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="61"/>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
+      <c r="AL5" s="61"/>
+      <c r="AM5" s="61"/>
+      <c r="AN5" s="61"/>
+      <c r="AO5" s="61"/>
+      <c r="AP5" s="61"/>
+      <c r="AQ5" s="61"/>
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="61"/>
+      <c r="AT5" s="61"/>
+      <c r="AU5" s="61"/>
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="61"/>
+      <c r="AX5" s="61"/>
+      <c r="AY5" s="61"/>
+      <c r="AZ5" s="61"/>
+      <c r="BA5" s="61"/>
+      <c r="BB5" s="61"/>
+      <c r="BC5" s="61"/>
+      <c r="BD5" s="61"/>
+      <c r="BE5" s="61"/>
+      <c r="BF5" s="61"/>
+      <c r="BG5" s="61"/>
+      <c r="BH5" s="61"/>
+      <c r="BI5" s="61"/>
+      <c r="BJ5" s="61"/>
+      <c r="BK5" s="61"/>
+      <c r="BL5" s="61"/>
+      <c r="BM5" s="61"/>
+      <c r="BN5" s="61"/>
+      <c r="BO5" s="61"/>
+      <c r="BP5" s="61"/>
+      <c r="BQ5" s="61"/>
+      <c r="BR5" s="61"/>
+      <c r="BS5" s="61"/>
+      <c r="BT5" s="61"/>
+      <c r="BU5" s="61"/>
+      <c r="BV5" s="61"/>
+      <c r="BW5" s="61"/>
+      <c r="BX5" s="61"/>
+      <c r="BY5" s="61"/>
     </row>
     <row r="6" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="41"/>
-      <c r="AG6" s="41"/>
-      <c r="AH6" s="41"/>
-      <c r="AI6" s="41"/>
-      <c r="AJ6" s="41"/>
-      <c r="AK6" s="41"/>
-      <c r="AL6" s="41"/>
-      <c r="AM6" s="41"/>
-      <c r="AN6" s="41"/>
-      <c r="AO6" s="41"/>
-      <c r="AP6" s="41"/>
-      <c r="AQ6" s="41"/>
-      <c r="AR6" s="41"/>
-      <c r="AS6" s="41"/>
-      <c r="AT6" s="41"/>
-      <c r="AU6" s="41"/>
-      <c r="AV6" s="41"/>
-      <c r="AW6" s="41"/>
-      <c r="AX6" s="41"/>
-      <c r="AY6" s="41"/>
-      <c r="AZ6" s="41"/>
-      <c r="BA6" s="41"/>
-      <c r="BB6" s="41"/>
-      <c r="BC6" s="41"/>
-      <c r="BD6" s="41"/>
-      <c r="BE6" s="41"/>
-      <c r="BF6" s="41"/>
-      <c r="BG6" s="41"/>
-      <c r="BH6" s="41"/>
-      <c r="BI6" s="41"/>
-      <c r="BJ6" s="41"/>
-      <c r="BK6" s="41"/>
-      <c r="BL6" s="41"/>
-      <c r="BM6" s="41"/>
-      <c r="BN6" s="41"/>
-      <c r="BO6" s="41"/>
-      <c r="BP6" s="41"/>
-      <c r="BQ6" s="41"/>
-      <c r="BR6" s="41"/>
-      <c r="BS6" s="41"/>
-      <c r="BT6" s="41"/>
-      <c r="BU6" s="41"/>
-      <c r="BV6" s="41"/>
-      <c r="BW6" s="41"/>
-      <c r="BX6" s="41"/>
-      <c r="BY6" s="41"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="62"/>
+      <c r="AA6" s="62"/>
+      <c r="AB6" s="62"/>
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="62"/>
+      <c r="AE6" s="62"/>
+      <c r="AF6" s="62"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="62"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="62"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="62"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="62"/>
+      <c r="AO6" s="62"/>
+      <c r="AP6" s="62"/>
+      <c r="AQ6" s="62"/>
+      <c r="AR6" s="62"/>
+      <c r="AS6" s="62"/>
+      <c r="AT6" s="62"/>
+      <c r="AU6" s="62"/>
+      <c r="AV6" s="62"/>
+      <c r="AW6" s="62"/>
+      <c r="AX6" s="62"/>
+      <c r="AY6" s="62"/>
+      <c r="AZ6" s="62"/>
+      <c r="BA6" s="62"/>
+      <c r="BB6" s="62"/>
+      <c r="BC6" s="62"/>
+      <c r="BD6" s="62"/>
+      <c r="BE6" s="62"/>
+      <c r="BF6" s="62"/>
+      <c r="BG6" s="62"/>
+      <c r="BH6" s="62"/>
+      <c r="BI6" s="62"/>
+      <c r="BJ6" s="62"/>
+      <c r="BK6" s="62"/>
+      <c r="BL6" s="62"/>
+      <c r="BM6" s="62"/>
+      <c r="BN6" s="62"/>
+      <c r="BO6" s="62"/>
+      <c r="BP6" s="62"/>
+      <c r="BQ6" s="62"/>
+      <c r="BR6" s="62"/>
+      <c r="BS6" s="62"/>
+      <c r="BT6" s="62"/>
+      <c r="BU6" s="62"/>
+      <c r="BV6" s="62"/>
+      <c r="BW6" s="62"/>
+      <c r="BX6" s="62"/>
+      <c r="BY6" s="62"/>
     </row>
     <row r="7" spans="1:77" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="50" t="s">
+      <c r="I7" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="50" t="s">
+      <c r="K7" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="50" t="s">
+      <c r="L7" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="56" t="s">
+      <c r="M7" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="56" t="s">
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="56" t="s">
+      <c r="S7" s="69"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="69"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="57"/>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="56" t="s">
+      <c r="X7" s="69"/>
+      <c r="Y7" s="69"/>
+      <c r="Z7" s="69"/>
+      <c r="AA7" s="70"/>
+      <c r="AB7" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="AC7" s="57"/>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="57"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="52" t="s">
+      <c r="AC7" s="69"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="69"/>
+      <c r="AF7" s="70"/>
+      <c r="AG7" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="AH7" s="52"/>
-      <c r="AI7" s="52"/>
-      <c r="AJ7" s="52"/>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="77" t="s">
+      <c r="AH7" s="60"/>
+      <c r="AI7" s="60"/>
+      <c r="AJ7" s="60"/>
+      <c r="AK7" s="60"/>
+      <c r="AL7" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="AM7" s="77"/>
-      <c r="AN7" s="77"/>
-      <c r="AO7" s="77"/>
-      <c r="AP7" s="77"/>
-      <c r="AQ7" s="77" t="s">
+      <c r="AM7" s="59"/>
+      <c r="AN7" s="59"/>
+      <c r="AO7" s="59"/>
+      <c r="AP7" s="59"/>
+      <c r="AQ7" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="AR7" s="77"/>
-      <c r="AS7" s="77"/>
-      <c r="AT7" s="77"/>
-      <c r="AU7" s="77"/>
-      <c r="AV7" s="77" t="s">
+      <c r="AR7" s="59"/>
+      <c r="AS7" s="59"/>
+      <c r="AT7" s="59"/>
+      <c r="AU7" s="59"/>
+      <c r="AV7" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="AW7" s="77"/>
-      <c r="AX7" s="77"/>
-      <c r="AY7" s="77"/>
-      <c r="AZ7" s="77"/>
-      <c r="BA7" s="53" t="s">
+      <c r="AW7" s="59"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="59"/>
+      <c r="AZ7" s="59"/>
+      <c r="BA7" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="BB7" s="54"/>
-      <c r="BC7" s="54"/>
-      <c r="BD7" s="54"/>
-      <c r="BE7" s="55"/>
-      <c r="BF7" s="52" t="s">
+      <c r="BB7" s="66"/>
+      <c r="BC7" s="66"/>
+      <c r="BD7" s="66"/>
+      <c r="BE7" s="67"/>
+      <c r="BF7" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="BG7" s="52"/>
-      <c r="BH7" s="52"/>
-      <c r="BI7" s="52"/>
-      <c r="BJ7" s="52"/>
-      <c r="BK7" s="77" t="s">
+      <c r="BG7" s="60"/>
+      <c r="BH7" s="60"/>
+      <c r="BI7" s="60"/>
+      <c r="BJ7" s="60"/>
+      <c r="BK7" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="BL7" s="77"/>
-      <c r="BM7" s="77"/>
-      <c r="BN7" s="77"/>
-      <c r="BO7" s="77"/>
-      <c r="BP7" s="77" t="s">
+      <c r="BL7" s="59"/>
+      <c r="BM7" s="59"/>
+      <c r="BN7" s="59"/>
+      <c r="BO7" s="59"/>
+      <c r="BP7" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="BQ7" s="77"/>
-      <c r="BR7" s="77"/>
-      <c r="BS7" s="77"/>
-      <c r="BT7" s="77"/>
-      <c r="BU7" s="52" t="s">
+      <c r="BQ7" s="59"/>
+      <c r="BR7" s="59"/>
+      <c r="BS7" s="59"/>
+      <c r="BT7" s="59"/>
+      <c r="BU7" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="BV7" s="52"/>
-      <c r="BW7" s="52"/>
-      <c r="BX7" s="52"/>
-      <c r="BY7" s="52"/>
+      <c r="BV7" s="60"/>
+      <c r="BW7" s="60"/>
+      <c r="BX7" s="60"/>
+      <c r="BY7" s="60"/>
     </row>
     <row r="8" spans="1:77" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
       <c r="M8" s="24" t="s">
         <v>75</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="BE8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="BF8" s="80" t="s">
+      <c r="BF8" s="55" t="s">
         <v>75</v>
       </c>
       <c r="BG8" s="24" t="s">
@@ -2500,7 +2500,7 @@
       <c r="BC9" s="26"/>
       <c r="BD9" s="26"/>
       <c r="BE9" s="27"/>
-      <c r="BF9" s="81"/>
+      <c r="BF9" s="56"/>
       <c r="BG9" s="26"/>
       <c r="BH9" s="26"/>
       <c r="BI9" s="26"/>
@@ -2519,7 +2519,7 @@
       <c r="BV9" s="26"/>
       <c r="BW9" s="26"/>
       <c r="BX9" s="26"/>
-      <c r="BY9" s="83"/>
+      <c r="BY9" s="58"/>
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -2606,7 +2606,7 @@
       <c r="BC10" s="26"/>
       <c r="BD10" s="26"/>
       <c r="BE10" s="27"/>
-      <c r="BF10" s="81"/>
+      <c r="BF10" s="56"/>
       <c r="BG10" s="26"/>
       <c r="BH10" s="26"/>
       <c r="BI10" s="26"/>
@@ -2625,7 +2625,7 @@
       <c r="BV10" s="26"/>
       <c r="BW10" s="26"/>
       <c r="BX10" s="26"/>
-      <c r="BY10" s="83"/>
+      <c r="BY10" s="58"/>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -2702,7 +2702,7 @@
       <c r="BC11" s="26"/>
       <c r="BD11" s="26"/>
       <c r="BE11" s="27"/>
-      <c r="BF11" s="81"/>
+      <c r="BF11" s="56"/>
       <c r="BG11" s="26"/>
       <c r="BH11" s="26"/>
       <c r="BI11" s="26"/>
@@ -2721,7 +2721,7 @@
       <c r="BV11" s="26"/>
       <c r="BW11" s="26"/>
       <c r="BX11" s="26"/>
-      <c r="BY11" s="83"/>
+      <c r="BY11" s="58"/>
     </row>
     <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -2798,7 +2798,7 @@
       <c r="BC12" s="26"/>
       <c r="BD12" s="26"/>
       <c r="BE12" s="27"/>
-      <c r="BF12" s="81"/>
+      <c r="BF12" s="56"/>
       <c r="BG12" s="26"/>
       <c r="BH12" s="26"/>
       <c r="BI12" s="26"/>
@@ -2817,7 +2817,7 @@
       <c r="BV12" s="26"/>
       <c r="BW12" s="26"/>
       <c r="BX12" s="26"/>
-      <c r="BY12" s="83"/>
+      <c r="BY12" s="58"/>
     </row>
     <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2902,7 +2902,7 @@
       <c r="BC13" s="26"/>
       <c r="BD13" s="26"/>
       <c r="BE13" s="27"/>
-      <c r="BF13" s="81"/>
+      <c r="BF13" s="56"/>
       <c r="BG13" s="26"/>
       <c r="BH13" s="26"/>
       <c r="BI13" s="26"/>
@@ -2921,7 +2921,7 @@
       <c r="BV13" s="26"/>
       <c r="BW13" s="26"/>
       <c r="BX13" s="26"/>
-      <c r="BY13" s="83"/>
+      <c r="BY13" s="58"/>
     </row>
     <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -3004,7 +3004,7 @@
       <c r="BC14" s="26"/>
       <c r="BD14" s="26"/>
       <c r="BE14" s="27"/>
-      <c r="BF14" s="81"/>
+      <c r="BF14" s="56"/>
       <c r="BG14" s="26"/>
       <c r="BH14" s="26"/>
       <c r="BI14" s="26"/>
@@ -3023,7 +3023,7 @@
       <c r="BV14" s="26"/>
       <c r="BW14" s="26"/>
       <c r="BX14" s="26"/>
-      <c r="BY14" s="83"/>
+      <c r="BY14" s="58"/>
     </row>
     <row r="15" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -3106,7 +3106,7 @@
       <c r="BC15" s="26"/>
       <c r="BD15" s="26"/>
       <c r="BE15" s="27"/>
-      <c r="BF15" s="81"/>
+      <c r="BF15" s="56"/>
       <c r="BG15" s="26"/>
       <c r="BH15" s="26"/>
       <c r="BI15" s="26"/>
@@ -3125,7 +3125,7 @@
       <c r="BV15" s="26"/>
       <c r="BW15" s="26"/>
       <c r="BX15" s="26"/>
-      <c r="BY15" s="83"/>
+      <c r="BY15" s="58"/>
     </row>
     <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -3208,7 +3208,7 @@
       <c r="BC16" s="26"/>
       <c r="BD16" s="26"/>
       <c r="BE16" s="27"/>
-      <c r="BF16" s="81"/>
+      <c r="BF16" s="56"/>
       <c r="BG16" s="26"/>
       <c r="BH16" s="26"/>
       <c r="BI16" s="26"/>
@@ -3227,7 +3227,7 @@
       <c r="BV16" s="26"/>
       <c r="BW16" s="26"/>
       <c r="BX16" s="26"/>
-      <c r="BY16" s="83"/>
+      <c r="BY16" s="58"/>
     </row>
     <row r="17" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -3289,7 +3289,7 @@
       <c r="AJ17" s="34">
         <v>1</v>
       </c>
-      <c r="AK17" s="75">
+      <c r="AK17" s="51">
         <v>1</v>
       </c>
       <c r="AL17" s="25"/>
@@ -3312,7 +3312,7 @@
       <c r="BC17" s="26"/>
       <c r="BD17" s="26"/>
       <c r="BE17" s="27"/>
-      <c r="BF17" s="81"/>
+      <c r="BF17" s="56"/>
       <c r="BG17" s="26"/>
       <c r="BH17" s="26"/>
       <c r="BI17" s="26"/>
@@ -3331,7 +3331,7 @@
       <c r="BV17" s="26"/>
       <c r="BW17" s="26"/>
       <c r="BX17" s="26"/>
-      <c r="BY17" s="83"/>
+      <c r="BY17" s="58"/>
     </row>
     <row r="18" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -3414,7 +3414,7 @@
       <c r="BC18" s="26"/>
       <c r="BD18" s="26"/>
       <c r="BE18" s="27"/>
-      <c r="BF18" s="81"/>
+      <c r="BF18" s="56"/>
       <c r="BG18" s="26"/>
       <c r="BH18" s="26"/>
       <c r="BI18" s="26"/>
@@ -3433,7 +3433,7 @@
       <c r="BV18" s="26"/>
       <c r="BW18" s="26"/>
       <c r="BX18" s="26"/>
-      <c r="BY18" s="83"/>
+      <c r="BY18" s="58"/>
     </row>
     <row r="19" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -3516,7 +3516,7 @@
       <c r="BC19" s="26"/>
       <c r="BD19" s="26"/>
       <c r="BE19" s="27"/>
-      <c r="BF19" s="81"/>
+      <c r="BF19" s="56"/>
       <c r="BG19" s="26"/>
       <c r="BH19" s="26"/>
       <c r="BI19" s="26"/>
@@ -3535,7 +3535,7 @@
       <c r="BV19" s="26"/>
       <c r="BW19" s="26"/>
       <c r="BX19" s="26"/>
-      <c r="BY19" s="83"/>
+      <c r="BY19" s="58"/>
     </row>
     <row r="20" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -3606,7 +3606,7 @@
       <c r="BC20" s="26"/>
       <c r="BD20" s="26"/>
       <c r="BE20" s="27"/>
-      <c r="BF20" s="81"/>
+      <c r="BF20" s="56"/>
       <c r="BG20" s="26"/>
       <c r="BH20" s="26"/>
       <c r="BI20" s="26"/>
@@ -3625,7 +3625,7 @@
       <c r="BV20" s="26"/>
       <c r="BW20" s="26"/>
       <c r="BX20" s="26"/>
-      <c r="BY20" s="83"/>
+      <c r="BY20" s="58"/>
     </row>
     <row r="21" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -3698,7 +3698,7 @@
       <c r="BC21" s="26"/>
       <c r="BD21" s="26"/>
       <c r="BE21" s="27"/>
-      <c r="BF21" s="81"/>
+      <c r="BF21" s="56"/>
       <c r="BG21" s="26"/>
       <c r="BH21" s="26"/>
       <c r="BI21" s="26"/>
@@ -3717,7 +3717,7 @@
       <c r="BV21" s="26"/>
       <c r="BW21" s="26"/>
       <c r="BX21" s="26"/>
-      <c r="BY21" s="83"/>
+      <c r="BY21" s="58"/>
     </row>
     <row r="22" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -3804,7 +3804,7 @@
       <c r="BC22" s="26"/>
       <c r="BD22" s="26"/>
       <c r="BE22" s="27"/>
-      <c r="BF22" s="81"/>
+      <c r="BF22" s="56"/>
       <c r="BG22" s="26"/>
       <c r="BH22" s="26"/>
       <c r="BI22" s="26"/>
@@ -3823,7 +3823,7 @@
       <c r="BV22" s="26"/>
       <c r="BW22" s="26"/>
       <c r="BX22" s="26"/>
-      <c r="BY22" s="83"/>
+      <c r="BY22" s="58"/>
     </row>
     <row r="23" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -3900,7 +3900,7 @@
       <c r="BC23" s="26"/>
       <c r="BD23" s="26"/>
       <c r="BE23" s="27"/>
-      <c r="BF23" s="81"/>
+      <c r="BF23" s="56"/>
       <c r="BG23" s="26"/>
       <c r="BH23" s="26"/>
       <c r="BI23" s="26"/>
@@ -3919,7 +3919,7 @@
       <c r="BV23" s="26"/>
       <c r="BW23" s="26"/>
       <c r="BX23" s="26"/>
-      <c r="BY23" s="83"/>
+      <c r="BY23" s="58"/>
     </row>
     <row r="24" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -3996,7 +3996,7 @@
       <c r="BC24" s="26"/>
       <c r="BD24" s="26"/>
       <c r="BE24" s="27"/>
-      <c r="BF24" s="81"/>
+      <c r="BF24" s="56"/>
       <c r="BG24" s="26"/>
       <c r="BH24" s="26"/>
       <c r="BI24" s="26"/>
@@ -4015,7 +4015,7 @@
       <c r="BV24" s="26"/>
       <c r="BW24" s="26"/>
       <c r="BX24" s="26"/>
-      <c r="BY24" s="83"/>
+      <c r="BY24" s="58"/>
     </row>
     <row r="25" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -4098,7 +4098,7 @@
       <c r="BC25" s="26"/>
       <c r="BD25" s="26"/>
       <c r="BE25" s="27"/>
-      <c r="BF25" s="81"/>
+      <c r="BF25" s="56"/>
       <c r="BG25" s="26"/>
       <c r="BH25" s="26"/>
       <c r="BI25" s="26"/>
@@ -4117,7 +4117,7 @@
       <c r="BV25" s="26"/>
       <c r="BW25" s="26"/>
       <c r="BX25" s="26"/>
-      <c r="BY25" s="83"/>
+      <c r="BY25" s="58"/>
     </row>
     <row r="26" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -4200,7 +4200,7 @@
       <c r="BC26" s="26"/>
       <c r="BD26" s="26"/>
       <c r="BE26" s="27"/>
-      <c r="BF26" s="81"/>
+      <c r="BF26" s="56"/>
       <c r="BG26" s="26"/>
       <c r="BH26" s="26"/>
       <c r="BI26" s="26"/>
@@ -4219,7 +4219,7 @@
       <c r="BV26" s="26"/>
       <c r="BW26" s="26"/>
       <c r="BX26" s="26"/>
-      <c r="BY26" s="83"/>
+      <c r="BY26" s="58"/>
     </row>
     <row r="27" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -4302,7 +4302,7 @@
       <c r="BC27" s="26"/>
       <c r="BD27" s="26"/>
       <c r="BE27" s="27"/>
-      <c r="BF27" s="81"/>
+      <c r="BF27" s="56"/>
       <c r="BG27" s="26"/>
       <c r="BH27" s="26"/>
       <c r="BI27" s="26"/>
@@ -4321,7 +4321,7 @@
       <c r="BV27" s="26"/>
       <c r="BW27" s="26"/>
       <c r="BX27" s="26"/>
-      <c r="BY27" s="83"/>
+      <c r="BY27" s="58"/>
     </row>
     <row r="28" spans="1:77" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -4404,7 +4404,7 @@
       <c r="BC28" s="26"/>
       <c r="BD28" s="26"/>
       <c r="BE28" s="27"/>
-      <c r="BF28" s="81"/>
+      <c r="BF28" s="56"/>
       <c r="BG28" s="26"/>
       <c r="BH28" s="26"/>
       <c r="BI28" s="26"/>
@@ -4423,7 +4423,7 @@
       <c r="BV28" s="26"/>
       <c r="BW28" s="26"/>
       <c r="BX28" s="26"/>
-      <c r="BY28" s="83"/>
+      <c r="BY28" s="58"/>
     </row>
     <row r="29" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -4506,7 +4506,7 @@
       <c r="BC29" s="26"/>
       <c r="BD29" s="26"/>
       <c r="BE29" s="27"/>
-      <c r="BF29" s="81"/>
+      <c r="BF29" s="56"/>
       <c r="BG29" s="26"/>
       <c r="BH29" s="26"/>
       <c r="BI29" s="26"/>
@@ -4525,7 +4525,7 @@
       <c r="BV29" s="26"/>
       <c r="BW29" s="26"/>
       <c r="BX29" s="26"/>
-      <c r="BY29" s="83"/>
+      <c r="BY29" s="58"/>
     </row>
     <row r="30" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -4608,7 +4608,7 @@
       <c r="BC30" s="26"/>
       <c r="BD30" s="26"/>
       <c r="BE30" s="27"/>
-      <c r="BF30" s="81"/>
+      <c r="BF30" s="56"/>
       <c r="BG30" s="26"/>
       <c r="BH30" s="26"/>
       <c r="BI30" s="26"/>
@@ -4627,7 +4627,7 @@
       <c r="BV30" s="26"/>
       <c r="BW30" s="26"/>
       <c r="BX30" s="26"/>
-      <c r="BY30" s="83"/>
+      <c r="BY30" s="58"/>
     </row>
     <row r="31" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -4710,7 +4710,7 @@
       <c r="BC31" s="26"/>
       <c r="BD31" s="26"/>
       <c r="BE31" s="27"/>
-      <c r="BF31" s="81"/>
+      <c r="BF31" s="56"/>
       <c r="BG31" s="26"/>
       <c r="BH31" s="26"/>
       <c r="BI31" s="26"/>
@@ -4729,7 +4729,7 @@
       <c r="BV31" s="26"/>
       <c r="BW31" s="26"/>
       <c r="BX31" s="26"/>
-      <c r="BY31" s="83"/>
+      <c r="BY31" s="58"/>
     </row>
     <row r="32" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -4800,7 +4800,7 @@
       <c r="BC32" s="26"/>
       <c r="BD32" s="26"/>
       <c r="BE32" s="27"/>
-      <c r="BF32" s="81"/>
+      <c r="BF32" s="56"/>
       <c r="BG32" s="26"/>
       <c r="BH32" s="26"/>
       <c r="BI32" s="26"/>
@@ -4819,7 +4819,7 @@
       <c r="BV32" s="26"/>
       <c r="BW32" s="26"/>
       <c r="BX32" s="26"/>
-      <c r="BY32" s="83"/>
+      <c r="BY32" s="58"/>
     </row>
     <row r="33" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -4892,7 +4892,7 @@
       <c r="BC33" s="26"/>
       <c r="BD33" s="26"/>
       <c r="BE33" s="27"/>
-      <c r="BF33" s="81"/>
+      <c r="BF33" s="56"/>
       <c r="BG33" s="26"/>
       <c r="BH33" s="26"/>
       <c r="BI33" s="26"/>
@@ -4911,7 +4911,7 @@
       <c r="BV33" s="26"/>
       <c r="BW33" s="26"/>
       <c r="BX33" s="26"/>
-      <c r="BY33" s="83"/>
+      <c r="BY33" s="58"/>
     </row>
     <row r="34" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -5000,7 +5000,7 @@
       <c r="BC34" s="26"/>
       <c r="BD34" s="26"/>
       <c r="BE34" s="27"/>
-      <c r="BF34" s="81"/>
+      <c r="BF34" s="56"/>
       <c r="BG34" s="26"/>
       <c r="BH34" s="26"/>
       <c r="BI34" s="26"/>
@@ -5019,7 +5019,7 @@
       <c r="BV34" s="26"/>
       <c r="BW34" s="26"/>
       <c r="BX34" s="26"/>
-      <c r="BY34" s="83"/>
+      <c r="BY34" s="58"/>
     </row>
     <row r="35" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -5096,7 +5096,7 @@
       <c r="BC35" s="26"/>
       <c r="BD35" s="26"/>
       <c r="BE35" s="27"/>
-      <c r="BF35" s="81"/>
+      <c r="BF35" s="56"/>
       <c r="BG35" s="26"/>
       <c r="BH35" s="26"/>
       <c r="BI35" s="26"/>
@@ -5115,7 +5115,7 @@
       <c r="BV35" s="26"/>
       <c r="BW35" s="26"/>
       <c r="BX35" s="26"/>
-      <c r="BY35" s="83"/>
+      <c r="BY35" s="58"/>
     </row>
     <row r="36" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -5192,7 +5192,7 @@
       <c r="BC36" s="26"/>
       <c r="BD36" s="26"/>
       <c r="BE36" s="27"/>
-      <c r="BF36" s="81"/>
+      <c r="BF36" s="56"/>
       <c r="BG36" s="26"/>
       <c r="BH36" s="26"/>
       <c r="BI36" s="26"/>
@@ -5211,7 +5211,7 @@
       <c r="BV36" s="26"/>
       <c r="BW36" s="26"/>
       <c r="BX36" s="26"/>
-      <c r="BY36" s="83"/>
+      <c r="BY36" s="58"/>
     </row>
     <row r="37" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -5239,10 +5239,10 @@
         <v>9</v>
       </c>
       <c r="H37" s="32">
-        <v>43999</v>
+        <v>44005</v>
       </c>
       <c r="I37" s="32">
-        <v>44001</v>
+        <v>44007</v>
       </c>
       <c r="J37" s="32"/>
       <c r="K37" s="32"/>
@@ -5294,7 +5294,7 @@
       <c r="BC37" s="26"/>
       <c r="BD37" s="26"/>
       <c r="BE37" s="27"/>
-      <c r="BF37" s="81"/>
+      <c r="BF37" s="56"/>
       <c r="BG37" s="26"/>
       <c r="BH37" s="26"/>
       <c r="BI37" s="26"/>
@@ -5313,7 +5313,7 @@
       <c r="BV37" s="26"/>
       <c r="BW37" s="26"/>
       <c r="BX37" s="26"/>
-      <c r="BY37" s="83"/>
+      <c r="BY37" s="58"/>
     </row>
     <row r="38" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -5398,7 +5398,7 @@
       <c r="BC38" s="26"/>
       <c r="BD38" s="26"/>
       <c r="BE38" s="27"/>
-      <c r="BF38" s="81"/>
+      <c r="BF38" s="56"/>
       <c r="BG38" s="26"/>
       <c r="BH38" s="26"/>
       <c r="BI38" s="26"/>
@@ -5417,7 +5417,7 @@
       <c r="BV38" s="26"/>
       <c r="BW38" s="26"/>
       <c r="BX38" s="26"/>
-      <c r="BY38" s="83"/>
+      <c r="BY38" s="58"/>
     </row>
     <row r="39" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -5500,7 +5500,7 @@
       <c r="BC39" s="26"/>
       <c r="BD39" s="26"/>
       <c r="BE39" s="27"/>
-      <c r="BF39" s="81"/>
+      <c r="BF39" s="56"/>
       <c r="BG39" s="26"/>
       <c r="BH39" s="26"/>
       <c r="BI39" s="26"/>
@@ -5519,7 +5519,7 @@
       <c r="BV39" s="26"/>
       <c r="BW39" s="26"/>
       <c r="BX39" s="26"/>
-      <c r="BY39" s="83"/>
+      <c r="BY39" s="58"/>
     </row>
     <row r="40" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -5608,7 +5608,7 @@
       <c r="BC40" s="26"/>
       <c r="BD40" s="26"/>
       <c r="BE40" s="27"/>
-      <c r="BF40" s="81"/>
+      <c r="BF40" s="56"/>
       <c r="BG40" s="26"/>
       <c r="BH40" s="26"/>
       <c r="BI40" s="26"/>
@@ -5627,7 +5627,7 @@
       <c r="BV40" s="26"/>
       <c r="BW40" s="26"/>
       <c r="BX40" s="26"/>
-      <c r="BY40" s="83"/>
+      <c r="BY40" s="58"/>
     </row>
     <row r="41" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -5710,7 +5710,7 @@
       <c r="BC41" s="26"/>
       <c r="BD41" s="26"/>
       <c r="BE41" s="27"/>
-      <c r="BF41" s="81"/>
+      <c r="BF41" s="56"/>
       <c r="BG41" s="26"/>
       <c r="BH41" s="26"/>
       <c r="BI41" s="26"/>
@@ -5729,7 +5729,7 @@
       <c r="BV41" s="26"/>
       <c r="BW41" s="26"/>
       <c r="BX41" s="26"/>
-      <c r="BY41" s="83"/>
+      <c r="BY41" s="58"/>
     </row>
     <row r="42" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -5812,7 +5812,7 @@
       <c r="BC42" s="26"/>
       <c r="BD42" s="26"/>
       <c r="BE42" s="27"/>
-      <c r="BF42" s="81"/>
+      <c r="BF42" s="56"/>
       <c r="BG42" s="26"/>
       <c r="BH42" s="26"/>
       <c r="BI42" s="26"/>
@@ -5831,7 +5831,7 @@
       <c r="BV42" s="26"/>
       <c r="BW42" s="26"/>
       <c r="BX42" s="26"/>
-      <c r="BY42" s="83"/>
+      <c r="BY42" s="58"/>
     </row>
     <row r="43" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -5914,7 +5914,7 @@
       <c r="BC43" s="26"/>
       <c r="BD43" s="26"/>
       <c r="BE43" s="27"/>
-      <c r="BF43" s="81"/>
+      <c r="BF43" s="56"/>
       <c r="BG43" s="26"/>
       <c r="BH43" s="26"/>
       <c r="BI43" s="26"/>
@@ -5933,7 +5933,7 @@
       <c r="BV43" s="26"/>
       <c r="BW43" s="26"/>
       <c r="BX43" s="26"/>
-      <c r="BY43" s="83"/>
+      <c r="BY43" s="58"/>
     </row>
     <row r="44" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -6004,7 +6004,7 @@
       <c r="BC44" s="26"/>
       <c r="BD44" s="26"/>
       <c r="BE44" s="27"/>
-      <c r="BF44" s="81"/>
+      <c r="BF44" s="56"/>
       <c r="BG44" s="26"/>
       <c r="BH44" s="26"/>
       <c r="BI44" s="26"/>
@@ -6023,7 +6023,7 @@
       <c r="BV44" s="26"/>
       <c r="BW44" s="26"/>
       <c r="BX44" s="26"/>
-      <c r="BY44" s="83"/>
+      <c r="BY44" s="58"/>
     </row>
     <row r="45" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
@@ -6096,7 +6096,7 @@
       <c r="BC45" s="26"/>
       <c r="BD45" s="26"/>
       <c r="BE45" s="27"/>
-      <c r="BF45" s="81"/>
+      <c r="BF45" s="56"/>
       <c r="BG45" s="26"/>
       <c r="BH45" s="26"/>
       <c r="BI45" s="26"/>
@@ -6115,7 +6115,7 @@
       <c r="BV45" s="26"/>
       <c r="BW45" s="26"/>
       <c r="BX45" s="26"/>
-      <c r="BY45" s="83"/>
+      <c r="BY45" s="58"/>
     </row>
     <row r="46" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
@@ -6204,7 +6204,7 @@
       <c r="BC46" s="26"/>
       <c r="BD46" s="26"/>
       <c r="BE46" s="27"/>
-      <c r="BF46" s="81"/>
+      <c r="BF46" s="56"/>
       <c r="BG46" s="26"/>
       <c r="BH46" s="26"/>
       <c r="BI46" s="26"/>
@@ -6223,7 +6223,7 @@
       <c r="BV46" s="26"/>
       <c r="BW46" s="26"/>
       <c r="BX46" s="26"/>
-      <c r="BY46" s="83"/>
+      <c r="BY46" s="58"/>
     </row>
     <row r="47" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -6300,7 +6300,7 @@
       <c r="BC47" s="26"/>
       <c r="BD47" s="26"/>
       <c r="BE47" s="27"/>
-      <c r="BF47" s="81"/>
+      <c r="BF47" s="56"/>
       <c r="BG47" s="26"/>
       <c r="BH47" s="26"/>
       <c r="BI47" s="26"/>
@@ -6319,7 +6319,7 @@
       <c r="BV47" s="26"/>
       <c r="BW47" s="26"/>
       <c r="BX47" s="26"/>
-      <c r="BY47" s="83"/>
+      <c r="BY47" s="58"/>
     </row>
     <row r="48" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -6396,7 +6396,7 @@
       <c r="BC48" s="26"/>
       <c r="BD48" s="26"/>
       <c r="BE48" s="27"/>
-      <c r="BF48" s="81"/>
+      <c r="BF48" s="56"/>
       <c r="BG48" s="26"/>
       <c r="BH48" s="26"/>
       <c r="BI48" s="26"/>
@@ -6415,7 +6415,7 @@
       <c r="BV48" s="26"/>
       <c r="BW48" s="26"/>
       <c r="BX48" s="26"/>
-      <c r="BY48" s="83"/>
+      <c r="BY48" s="58"/>
     </row>
     <row r="49" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -6500,7 +6500,7 @@
       <c r="BC49" s="26"/>
       <c r="BD49" s="26"/>
       <c r="BE49" s="27"/>
-      <c r="BF49" s="81"/>
+      <c r="BF49" s="56"/>
       <c r="BG49" s="26"/>
       <c r="BH49" s="26"/>
       <c r="BI49" s="26"/>
@@ -6519,7 +6519,7 @@
       <c r="BV49" s="26"/>
       <c r="BW49" s="26"/>
       <c r="BX49" s="26"/>
-      <c r="BY49" s="83"/>
+      <c r="BY49" s="58"/>
     </row>
     <row r="50" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -6604,7 +6604,7 @@
       <c r="BC50" s="26"/>
       <c r="BD50" s="26"/>
       <c r="BE50" s="27"/>
-      <c r="BF50" s="81"/>
+      <c r="BF50" s="56"/>
       <c r="BG50" s="26"/>
       <c r="BH50" s="26"/>
       <c r="BI50" s="26"/>
@@ -6623,7 +6623,7 @@
       <c r="BV50" s="26"/>
       <c r="BW50" s="26"/>
       <c r="BX50" s="26"/>
-      <c r="BY50" s="83"/>
+      <c r="BY50" s="58"/>
     </row>
     <row r="51" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -6708,7 +6708,7 @@
       <c r="BC51" s="26"/>
       <c r="BD51" s="26"/>
       <c r="BE51" s="27"/>
-      <c r="BF51" s="81"/>
+      <c r="BF51" s="56"/>
       <c r="BG51" s="26"/>
       <c r="BH51" s="26"/>
       <c r="BI51" s="26"/>
@@ -6727,7 +6727,7 @@
       <c r="BV51" s="26"/>
       <c r="BW51" s="26"/>
       <c r="BX51" s="26"/>
-      <c r="BY51" s="83"/>
+      <c r="BY51" s="58"/>
     </row>
     <row r="52" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
@@ -6810,7 +6810,7 @@
       <c r="BC52" s="26"/>
       <c r="BD52" s="26"/>
       <c r="BE52" s="27"/>
-      <c r="BF52" s="81"/>
+      <c r="BF52" s="56"/>
       <c r="BG52" s="26"/>
       <c r="BH52" s="26"/>
       <c r="BI52" s="26"/>
@@ -6829,7 +6829,7 @@
       <c r="BV52" s="26"/>
       <c r="BW52" s="26"/>
       <c r="BX52" s="26"/>
-      <c r="BY52" s="83"/>
+      <c r="BY52" s="58"/>
     </row>
     <row r="53" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -6912,7 +6912,7 @@
       <c r="BC53" s="26"/>
       <c r="BD53" s="26"/>
       <c r="BE53" s="27"/>
-      <c r="BF53" s="81"/>
+      <c r="BF53" s="56"/>
       <c r="BG53" s="26"/>
       <c r="BH53" s="26"/>
       <c r="BI53" s="26"/>
@@ -6931,7 +6931,7 @@
       <c r="BV53" s="26"/>
       <c r="BW53" s="26"/>
       <c r="BX53" s="26"/>
-      <c r="BY53" s="83"/>
+      <c r="BY53" s="58"/>
     </row>
     <row r="54" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
@@ -7014,7 +7014,7 @@
       <c r="BC54" s="26"/>
       <c r="BD54" s="26"/>
       <c r="BE54" s="27"/>
-      <c r="BF54" s="81"/>
+      <c r="BF54" s="56"/>
       <c r="BG54" s="26"/>
       <c r="BH54" s="26"/>
       <c r="BI54" s="26"/>
@@ -7033,7 +7033,7 @@
       <c r="BV54" s="26"/>
       <c r="BW54" s="26"/>
       <c r="BX54" s="26"/>
-      <c r="BY54" s="83"/>
+      <c r="BY54" s="58"/>
     </row>
     <row r="55" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
@@ -7116,7 +7116,7 @@
       <c r="BC55" s="26"/>
       <c r="BD55" s="26"/>
       <c r="BE55" s="27"/>
-      <c r="BF55" s="81"/>
+      <c r="BF55" s="56"/>
       <c r="BG55" s="26"/>
       <c r="BH55" s="26"/>
       <c r="BI55" s="26"/>
@@ -7135,7 +7135,7 @@
       <c r="BV55" s="26"/>
       <c r="BW55" s="26"/>
       <c r="BX55" s="26"/>
-      <c r="BY55" s="83"/>
+      <c r="BY55" s="58"/>
     </row>
     <row r="56" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
@@ -7206,7 +7206,7 @@
       <c r="BC56" s="26"/>
       <c r="BD56" s="26"/>
       <c r="BE56" s="27"/>
-      <c r="BF56" s="81"/>
+      <c r="BF56" s="56"/>
       <c r="BG56" s="26"/>
       <c r="BH56" s="26"/>
       <c r="BI56" s="26"/>
@@ -7225,7 +7225,7 @@
       <c r="BV56" s="26"/>
       <c r="BW56" s="26"/>
       <c r="BX56" s="26"/>
-      <c r="BY56" s="83"/>
+      <c r="BY56" s="58"/>
     </row>
     <row r="57" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -7300,7 +7300,7 @@
       <c r="BC57" s="26"/>
       <c r="BD57" s="26"/>
       <c r="BE57" s="27"/>
-      <c r="BF57" s="81"/>
+      <c r="BF57" s="56"/>
       <c r="BG57" s="26"/>
       <c r="BH57" s="26"/>
       <c r="BI57" s="26"/>
@@ -7319,7 +7319,7 @@
       <c r="BV57" s="26"/>
       <c r="BW57" s="26"/>
       <c r="BX57" s="26"/>
-      <c r="BY57" s="83"/>
+      <c r="BY57" s="58"/>
     </row>
     <row r="58" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
@@ -7406,7 +7406,7 @@
       <c r="BC58" s="26"/>
       <c r="BD58" s="26"/>
       <c r="BE58" s="27"/>
-      <c r="BF58" s="81"/>
+      <c r="BF58" s="56"/>
       <c r="BG58" s="26"/>
       <c r="BH58" s="26"/>
       <c r="BI58" s="26"/>
@@ -7425,7 +7425,7 @@
       <c r="BV58" s="26"/>
       <c r="BW58" s="26"/>
       <c r="BX58" s="26"/>
-      <c r="BY58" s="83"/>
+      <c r="BY58" s="58"/>
     </row>
     <row r="59" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
@@ -7502,7 +7502,7 @@
       <c r="BC59" s="26"/>
       <c r="BD59" s="26"/>
       <c r="BE59" s="27"/>
-      <c r="BF59" s="81"/>
+      <c r="BF59" s="56"/>
       <c r="BG59" s="26"/>
       <c r="BH59" s="26"/>
       <c r="BI59" s="26"/>
@@ -7521,7 +7521,7 @@
       <c r="BV59" s="26"/>
       <c r="BW59" s="26"/>
       <c r="BX59" s="26"/>
-      <c r="BY59" s="83"/>
+      <c r="BY59" s="58"/>
     </row>
     <row r="60" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -7598,7 +7598,7 @@
       <c r="BC60" s="26"/>
       <c r="BD60" s="26"/>
       <c r="BE60" s="27"/>
-      <c r="BF60" s="81"/>
+      <c r="BF60" s="56"/>
       <c r="BG60" s="26"/>
       <c r="BH60" s="26"/>
       <c r="BI60" s="26"/>
@@ -7617,7 +7617,7 @@
       <c r="BV60" s="26"/>
       <c r="BW60" s="26"/>
       <c r="BX60" s="26"/>
-      <c r="BY60" s="83"/>
+      <c r="BY60" s="58"/>
     </row>
     <row r="61" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
@@ -7700,7 +7700,7 @@
       <c r="BC61" s="26"/>
       <c r="BD61" s="26"/>
       <c r="BE61" s="27"/>
-      <c r="BF61" s="81"/>
+      <c r="BF61" s="56"/>
       <c r="BG61" s="26"/>
       <c r="BH61" s="26"/>
       <c r="BI61" s="26"/>
@@ -7719,7 +7719,7 @@
       <c r="BV61" s="26"/>
       <c r="BW61" s="26"/>
       <c r="BX61" s="26"/>
-      <c r="BY61" s="83"/>
+      <c r="BY61" s="58"/>
     </row>
     <row r="62" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
@@ -7804,7 +7804,7 @@
       <c r="BC62" s="26"/>
       <c r="BD62" s="26"/>
       <c r="BE62" s="27"/>
-      <c r="BF62" s="81"/>
+      <c r="BF62" s="56"/>
       <c r="BG62" s="26"/>
       <c r="BH62" s="26"/>
       <c r="BI62" s="26"/>
@@ -7823,7 +7823,7 @@
       <c r="BV62" s="26"/>
       <c r="BW62" s="26"/>
       <c r="BX62" s="26"/>
-      <c r="BY62" s="83"/>
+      <c r="BY62" s="58"/>
     </row>
     <row r="63" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
@@ -7906,7 +7906,7 @@
       <c r="BC63" s="26"/>
       <c r="BD63" s="26"/>
       <c r="BE63" s="27"/>
-      <c r="BF63" s="81"/>
+      <c r="BF63" s="56"/>
       <c r="BG63" s="26"/>
       <c r="BH63" s="26"/>
       <c r="BI63" s="26"/>
@@ -7925,7 +7925,7 @@
       <c r="BV63" s="26"/>
       <c r="BW63" s="26"/>
       <c r="BX63" s="26"/>
-      <c r="BY63" s="83"/>
+      <c r="BY63" s="58"/>
     </row>
     <row r="64" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
@@ -8010,7 +8010,7 @@
       <c r="BC64" s="26"/>
       <c r="BD64" s="26"/>
       <c r="BE64" s="27"/>
-      <c r="BF64" s="81"/>
+      <c r="BF64" s="56"/>
       <c r="BG64" s="26"/>
       <c r="BH64" s="26"/>
       <c r="BI64" s="26"/>
@@ -8029,7 +8029,7 @@
       <c r="BV64" s="26"/>
       <c r="BW64" s="26"/>
       <c r="BX64" s="26"/>
-      <c r="BY64" s="83"/>
+      <c r="BY64" s="58"/>
     </row>
     <row r="65" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -8112,7 +8112,7 @@
       <c r="BC65" s="26"/>
       <c r="BD65" s="26"/>
       <c r="BE65" s="27"/>
-      <c r="BF65" s="81"/>
+      <c r="BF65" s="56"/>
       <c r="BG65" s="26"/>
       <c r="BH65" s="26"/>
       <c r="BI65" s="26"/>
@@ -8131,7 +8131,7 @@
       <c r="BV65" s="26"/>
       <c r="BW65" s="26"/>
       <c r="BX65" s="26"/>
-      <c r="BY65" s="83"/>
+      <c r="BY65" s="58"/>
     </row>
     <row r="66" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -8214,7 +8214,7 @@
       <c r="BC66" s="26"/>
       <c r="BD66" s="26"/>
       <c r="BE66" s="27"/>
-      <c r="BF66" s="81"/>
+      <c r="BF66" s="56"/>
       <c r="BG66" s="26"/>
       <c r="BH66" s="26"/>
       <c r="BI66" s="26"/>
@@ -8233,7 +8233,7 @@
       <c r="BV66" s="26"/>
       <c r="BW66" s="26"/>
       <c r="BX66" s="26"/>
-      <c r="BY66" s="83"/>
+      <c r="BY66" s="58"/>
     </row>
     <row r="67" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
@@ -8316,7 +8316,7 @@
       <c r="BC67" s="26"/>
       <c r="BD67" s="26"/>
       <c r="BE67" s="27"/>
-      <c r="BF67" s="81"/>
+      <c r="BF67" s="56"/>
       <c r="BG67" s="26"/>
       <c r="BH67" s="26"/>
       <c r="BI67" s="26"/>
@@ -8335,7 +8335,7 @@
       <c r="BV67" s="26"/>
       <c r="BW67" s="26"/>
       <c r="BX67" s="26"/>
-      <c r="BY67" s="83"/>
+      <c r="BY67" s="58"/>
     </row>
     <row r="68" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
@@ -8406,7 +8406,7 @@
       <c r="BC68" s="26"/>
       <c r="BD68" s="26"/>
       <c r="BE68" s="27"/>
-      <c r="BF68" s="81"/>
+      <c r="BF68" s="56"/>
       <c r="BG68" s="26"/>
       <c r="BH68" s="26"/>
       <c r="BI68" s="26"/>
@@ -8425,7 +8425,7 @@
       <c r="BV68" s="26"/>
       <c r="BW68" s="26"/>
       <c r="BX68" s="26"/>
-      <c r="BY68" s="83"/>
+      <c r="BY68" s="58"/>
     </row>
     <row r="69" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
@@ -8500,7 +8500,7 @@
       <c r="BC69" s="26"/>
       <c r="BD69" s="26"/>
       <c r="BE69" s="27"/>
-      <c r="BF69" s="81"/>
+      <c r="BF69" s="56"/>
       <c r="BG69" s="26"/>
       <c r="BH69" s="26"/>
       <c r="BI69" s="26"/>
@@ -8519,7 +8519,7 @@
       <c r="BV69" s="26"/>
       <c r="BW69" s="26"/>
       <c r="BX69" s="26"/>
-      <c r="BY69" s="83"/>
+      <c r="BY69" s="58"/>
     </row>
     <row r="70" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
@@ -8606,7 +8606,7 @@
       <c r="BC70" s="26"/>
       <c r="BD70" s="26"/>
       <c r="BE70" s="27"/>
-      <c r="BF70" s="81"/>
+      <c r="BF70" s="56"/>
       <c r="BG70" s="26"/>
       <c r="BH70" s="26"/>
       <c r="BI70" s="26"/>
@@ -8625,7 +8625,7 @@
       <c r="BV70" s="26"/>
       <c r="BW70" s="26"/>
       <c r="BX70" s="26"/>
-      <c r="BY70" s="83"/>
+      <c r="BY70" s="58"/>
     </row>
     <row r="71" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -8702,7 +8702,7 @@
       <c r="BC71" s="26"/>
       <c r="BD71" s="26"/>
       <c r="BE71" s="27"/>
-      <c r="BF71" s="81"/>
+      <c r="BF71" s="56"/>
       <c r="BG71" s="26"/>
       <c r="BH71" s="26"/>
       <c r="BI71" s="26"/>
@@ -8721,7 +8721,7 @@
       <c r="BV71" s="26"/>
       <c r="BW71" s="26"/>
       <c r="BX71" s="26"/>
-      <c r="BY71" s="83"/>
+      <c r="BY71" s="58"/>
     </row>
     <row r="72" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
@@ -8798,7 +8798,7 @@
       <c r="BC72" s="26"/>
       <c r="BD72" s="26"/>
       <c r="BE72" s="27"/>
-      <c r="BF72" s="81"/>
+      <c r="BF72" s="56"/>
       <c r="BG72" s="26"/>
       <c r="BH72" s="26"/>
       <c r="BI72" s="26"/>
@@ -8817,7 +8817,7 @@
       <c r="BV72" s="26"/>
       <c r="BW72" s="26"/>
       <c r="BX72" s="26"/>
-      <c r="BY72" s="83"/>
+      <c r="BY72" s="58"/>
     </row>
     <row r="73" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
@@ -8900,7 +8900,7 @@
       <c r="BC73" s="26"/>
       <c r="BD73" s="26"/>
       <c r="BE73" s="27"/>
-      <c r="BF73" s="81"/>
+      <c r="BF73" s="56"/>
       <c r="BG73" s="26"/>
       <c r="BH73" s="26"/>
       <c r="BI73" s="26"/>
@@ -8919,7 +8919,7 @@
       <c r="BV73" s="26"/>
       <c r="BW73" s="26"/>
       <c r="BX73" s="26"/>
-      <c r="BY73" s="83"/>
+      <c r="BY73" s="58"/>
     </row>
     <row r="74" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
@@ -9004,7 +9004,7 @@
       <c r="BC74" s="26"/>
       <c r="BD74" s="26"/>
       <c r="BE74" s="27"/>
-      <c r="BF74" s="81"/>
+      <c r="BF74" s="56"/>
       <c r="BG74" s="26"/>
       <c r="BH74" s="26"/>
       <c r="BI74" s="26"/>
@@ -9023,7 +9023,7 @@
       <c r="BV74" s="26"/>
       <c r="BW74" s="26"/>
       <c r="BX74" s="26"/>
-      <c r="BY74" s="83"/>
+      <c r="BY74" s="58"/>
     </row>
     <row r="75" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
@@ -9106,7 +9106,7 @@
       <c r="BC75" s="26"/>
       <c r="BD75" s="26"/>
       <c r="BE75" s="27"/>
-      <c r="BF75" s="81"/>
+      <c r="BF75" s="56"/>
       <c r="BG75" s="26"/>
       <c r="BH75" s="26"/>
       <c r="BI75" s="26"/>
@@ -9125,7 +9125,7 @@
       <c r="BV75" s="26"/>
       <c r="BW75" s="26"/>
       <c r="BX75" s="26"/>
-      <c r="BY75" s="83"/>
+      <c r="BY75" s="58"/>
     </row>
     <row r="76" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
@@ -9210,7 +9210,7 @@
       <c r="BC76" s="26"/>
       <c r="BD76" s="26"/>
       <c r="BE76" s="27"/>
-      <c r="BF76" s="81"/>
+      <c r="BF76" s="56"/>
       <c r="BG76" s="26"/>
       <c r="BH76" s="26"/>
       <c r="BI76" s="26"/>
@@ -9229,7 +9229,7 @@
       <c r="BV76" s="26"/>
       <c r="BW76" s="26"/>
       <c r="BX76" s="26"/>
-      <c r="BY76" s="83"/>
+      <c r="BY76" s="58"/>
     </row>
     <row r="77" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
@@ -9311,7 +9311,7 @@
       <c r="BC77" s="26"/>
       <c r="BD77" s="26"/>
       <c r="BE77" s="27"/>
-      <c r="BF77" s="81"/>
+      <c r="BF77" s="56"/>
       <c r="BG77" s="26"/>
       <c r="BH77" s="26"/>
       <c r="BI77" s="26"/>
@@ -9330,7 +9330,7 @@
       <c r="BV77" s="26"/>
       <c r="BW77" s="26"/>
       <c r="BX77" s="26"/>
-      <c r="BY77" s="83"/>
+      <c r="BY77" s="58"/>
     </row>
     <row r="78" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
@@ -9412,7 +9412,7 @@
       <c r="BC78" s="26"/>
       <c r="BD78" s="26"/>
       <c r="BE78" s="27"/>
-      <c r="BF78" s="81"/>
+      <c r="BF78" s="56"/>
       <c r="BG78" s="26"/>
       <c r="BH78" s="26"/>
       <c r="BI78" s="26"/>
@@ -9431,7 +9431,7 @@
       <c r="BV78" s="26"/>
       <c r="BW78" s="26"/>
       <c r="BX78" s="26"/>
-      <c r="BY78" s="83"/>
+      <c r="BY78" s="58"/>
     </row>
     <row r="79" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -9513,7 +9513,7 @@
       <c r="BC79" s="26"/>
       <c r="BD79" s="26"/>
       <c r="BE79" s="27"/>
-      <c r="BF79" s="81"/>
+      <c r="BF79" s="56"/>
       <c r="BG79" s="26"/>
       <c r="BH79" s="26"/>
       <c r="BI79" s="26"/>
@@ -9532,7 +9532,7 @@
       <c r="BV79" s="26"/>
       <c r="BW79" s="26"/>
       <c r="BX79" s="26"/>
-      <c r="BY79" s="83"/>
+      <c r="BY79" s="58"/>
     </row>
     <row r="80" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
@@ -9603,7 +9603,7 @@
       <c r="BC80" s="26"/>
       <c r="BD80" s="26"/>
       <c r="BE80" s="27"/>
-      <c r="BF80" s="81"/>
+      <c r="BF80" s="56"/>
       <c r="BG80" s="26"/>
       <c r="BH80" s="26"/>
       <c r="BI80" s="26"/>
@@ -9622,7 +9622,7 @@
       <c r="BV80" s="26"/>
       <c r="BW80" s="26"/>
       <c r="BX80" s="26"/>
-      <c r="BY80" s="83"/>
+      <c r="BY80" s="58"/>
     </row>
     <row r="81" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
@@ -9695,7 +9695,7 @@
       <c r="BC81" s="26"/>
       <c r="BD81" s="26"/>
       <c r="BE81" s="27"/>
-      <c r="BF81" s="81"/>
+      <c r="BF81" s="56"/>
       <c r="BG81" s="26"/>
       <c r="BH81" s="26"/>
       <c r="BI81" s="26"/>
@@ -9714,7 +9714,7 @@
       <c r="BV81" s="26"/>
       <c r="BW81" s="26"/>
       <c r="BX81" s="26"/>
-      <c r="BY81" s="83"/>
+      <c r="BY81" s="58"/>
     </row>
     <row r="82" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
@@ -9797,7 +9797,7 @@
       <c r="BC82" s="26"/>
       <c r="BD82" s="26"/>
       <c r="BE82" s="27"/>
-      <c r="BF82" s="81"/>
+      <c r="BF82" s="56"/>
       <c r="BG82" s="26"/>
       <c r="BH82" s="26"/>
       <c r="BI82" s="26"/>
@@ -9816,7 +9816,7 @@
       <c r="BV82" s="26"/>
       <c r="BW82" s="26"/>
       <c r="BX82" s="26"/>
-      <c r="BY82" s="83"/>
+      <c r="BY82" s="58"/>
     </row>
     <row r="83" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
@@ -9893,7 +9893,7 @@
       <c r="BC83" s="26"/>
       <c r="BD83" s="26"/>
       <c r="BE83" s="27"/>
-      <c r="BF83" s="81"/>
+      <c r="BF83" s="56"/>
       <c r="BG83" s="26"/>
       <c r="BH83" s="26"/>
       <c r="BI83" s="26"/>
@@ -9912,7 +9912,7 @@
       <c r="BV83" s="26"/>
       <c r="BW83" s="26"/>
       <c r="BX83" s="26"/>
-      <c r="BY83" s="83"/>
+      <c r="BY83" s="58"/>
     </row>
     <row r="84" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
@@ -9989,7 +9989,7 @@
       <c r="BC84" s="26"/>
       <c r="BD84" s="26"/>
       <c r="BE84" s="27"/>
-      <c r="BF84" s="81"/>
+      <c r="BF84" s="56"/>
       <c r="BG84" s="26"/>
       <c r="BH84" s="26"/>
       <c r="BI84" s="26"/>
@@ -10008,7 +10008,7 @@
       <c r="BV84" s="26"/>
       <c r="BW84" s="26"/>
       <c r="BX84" s="26"/>
-      <c r="BY84" s="83"/>
+      <c r="BY84" s="58"/>
     </row>
     <row r="85" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
@@ -10091,7 +10091,7 @@
       <c r="BC85" s="26"/>
       <c r="BD85" s="26"/>
       <c r="BE85" s="27"/>
-      <c r="BF85" s="81"/>
+      <c r="BF85" s="56"/>
       <c r="BG85" s="26"/>
       <c r="BH85" s="26"/>
       <c r="BI85" s="26"/>
@@ -10110,7 +10110,7 @@
       <c r="BV85" s="26"/>
       <c r="BW85" s="26"/>
       <c r="BX85" s="26"/>
-      <c r="BY85" s="83"/>
+      <c r="BY85" s="58"/>
     </row>
     <row r="86" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
@@ -10195,7 +10195,7 @@
       <c r="BC86" s="26"/>
       <c r="BD86" s="26"/>
       <c r="BE86" s="27"/>
-      <c r="BF86" s="81"/>
+      <c r="BF86" s="56"/>
       <c r="BG86" s="26"/>
       <c r="BH86" s="26"/>
       <c r="BI86" s="26"/>
@@ -10214,7 +10214,7 @@
       <c r="BV86" s="26"/>
       <c r="BW86" s="26"/>
       <c r="BX86" s="26"/>
-      <c r="BY86" s="83"/>
+      <c r="BY86" s="58"/>
     </row>
     <row r="87" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
@@ -10299,7 +10299,7 @@
       <c r="BC87" s="26"/>
       <c r="BD87" s="26"/>
       <c r="BE87" s="27"/>
-      <c r="BF87" s="81"/>
+      <c r="BF87" s="56"/>
       <c r="BG87" s="26"/>
       <c r="BH87" s="26"/>
       <c r="BI87" s="26"/>
@@ -10318,7 +10318,7 @@
       <c r="BV87" s="26"/>
       <c r="BW87" s="26"/>
       <c r="BX87" s="26"/>
-      <c r="BY87" s="83"/>
+      <c r="BY87" s="58"/>
     </row>
     <row r="88" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -10403,7 +10403,7 @@
       </c>
       <c r="BD88" s="26"/>
       <c r="BE88" s="27"/>
-      <c r="BF88" s="81"/>
+      <c r="BF88" s="56"/>
       <c r="BG88" s="26"/>
       <c r="BH88" s="26"/>
       <c r="BI88" s="26"/>
@@ -10422,7 +10422,7 @@
       <c r="BV88" s="26"/>
       <c r="BW88" s="26"/>
       <c r="BX88" s="26"/>
-      <c r="BY88" s="83"/>
+      <c r="BY88" s="58"/>
     </row>
     <row r="89" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
@@ -10504,7 +10504,7 @@
       </c>
       <c r="BD89" s="26"/>
       <c r="BE89" s="27"/>
-      <c r="BF89" s="81"/>
+      <c r="BF89" s="56"/>
       <c r="BG89" s="26"/>
       <c r="BH89" s="26"/>
       <c r="BI89" s="26"/>
@@ -10523,7 +10523,7 @@
       <c r="BV89" s="26"/>
       <c r="BW89" s="26"/>
       <c r="BX89" s="26"/>
-      <c r="BY89" s="83"/>
+      <c r="BY89" s="58"/>
     </row>
     <row r="90" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -10605,7 +10605,7 @@
         <v>2</v>
       </c>
       <c r="BE90" s="27"/>
-      <c r="BF90" s="81"/>
+      <c r="BF90" s="56"/>
       <c r="BG90" s="26"/>
       <c r="BH90" s="26"/>
       <c r="BI90" s="26"/>
@@ -10624,7 +10624,7 @@
       <c r="BV90" s="26"/>
       <c r="BW90" s="26"/>
       <c r="BX90" s="26"/>
-      <c r="BY90" s="83"/>
+      <c r="BY90" s="58"/>
     </row>
     <row r="91" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
@@ -10706,7 +10706,7 @@
         <v>2</v>
       </c>
       <c r="BE91" s="27"/>
-      <c r="BF91" s="81"/>
+      <c r="BF91" s="56"/>
       <c r="BG91" s="26"/>
       <c r="BH91" s="26"/>
       <c r="BI91" s="26"/>
@@ -10725,7 +10725,7 @@
       <c r="BV91" s="26"/>
       <c r="BW91" s="26"/>
       <c r="BX91" s="26"/>
-      <c r="BY91" s="83"/>
+      <c r="BY91" s="58"/>
     </row>
     <row r="92" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
@@ -10796,7 +10796,7 @@
       <c r="BC92" s="26"/>
       <c r="BD92" s="26"/>
       <c r="BE92" s="27"/>
-      <c r="BF92" s="81"/>
+      <c r="BF92" s="56"/>
       <c r="BG92" s="26"/>
       <c r="BH92" s="26"/>
       <c r="BI92" s="26"/>
@@ -10815,7 +10815,7 @@
       <c r="BV92" s="26"/>
       <c r="BW92" s="26"/>
       <c r="BX92" s="26"/>
-      <c r="BY92" s="83"/>
+      <c r="BY92" s="58"/>
     </row>
     <row r="93" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
@@ -10888,7 +10888,7 @@
       <c r="BC93" s="26"/>
       <c r="BD93" s="26"/>
       <c r="BE93" s="27"/>
-      <c r="BF93" s="81"/>
+      <c r="BF93" s="56"/>
       <c r="BG93" s="26"/>
       <c r="BH93" s="26"/>
       <c r="BI93" s="26"/>
@@ -10907,7 +10907,7 @@
       <c r="BV93" s="26"/>
       <c r="BW93" s="26"/>
       <c r="BX93" s="26"/>
-      <c r="BY93" s="83"/>
+      <c r="BY93" s="58"/>
     </row>
     <row r="94" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
@@ -10990,7 +10990,7 @@
       <c r="BC94" s="26"/>
       <c r="BD94" s="26"/>
       <c r="BE94" s="27"/>
-      <c r="BF94" s="81"/>
+      <c r="BF94" s="56"/>
       <c r="BG94" s="26"/>
       <c r="BH94" s="26"/>
       <c r="BI94" s="26"/>
@@ -11009,7 +11009,7 @@
       <c r="BV94" s="26"/>
       <c r="BW94" s="26"/>
       <c r="BX94" s="26"/>
-      <c r="BY94" s="83"/>
+      <c r="BY94" s="58"/>
     </row>
     <row r="95" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
@@ -11086,7 +11086,7 @@
       <c r="BC95" s="26"/>
       <c r="BD95" s="26"/>
       <c r="BE95" s="27"/>
-      <c r="BF95" s="81"/>
+      <c r="BF95" s="56"/>
       <c r="BG95" s="26"/>
       <c r="BH95" s="26"/>
       <c r="BI95" s="26"/>
@@ -11105,7 +11105,7 @@
       <c r="BV95" s="26"/>
       <c r="BW95" s="26"/>
       <c r="BX95" s="26"/>
-      <c r="BY95" s="83"/>
+      <c r="BY95" s="58"/>
     </row>
     <row r="96" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
@@ -11182,7 +11182,7 @@
       <c r="BC96" s="26"/>
       <c r="BD96" s="26"/>
       <c r="BE96" s="27"/>
-      <c r="BF96" s="81"/>
+      <c r="BF96" s="56"/>
       <c r="BG96" s="26"/>
       <c r="BH96" s="26"/>
       <c r="BI96" s="26"/>
@@ -11201,7 +11201,7 @@
       <c r="BV96" s="26"/>
       <c r="BW96" s="26"/>
       <c r="BX96" s="26"/>
-      <c r="BY96" s="83"/>
+      <c r="BY96" s="58"/>
     </row>
     <row r="97" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
@@ -11284,7 +11284,7 @@
       <c r="BC97" s="26"/>
       <c r="BD97" s="26"/>
       <c r="BE97" s="27"/>
-      <c r="BF97" s="81"/>
+      <c r="BF97" s="56"/>
       <c r="BG97" s="26"/>
       <c r="BH97" s="26"/>
       <c r="BI97" s="26"/>
@@ -11303,7 +11303,7 @@
       <c r="BV97" s="26"/>
       <c r="BW97" s="26"/>
       <c r="BX97" s="26"/>
-      <c r="BY97" s="83"/>
+      <c r="BY97" s="58"/>
     </row>
     <row r="98" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
@@ -11386,7 +11386,7 @@
       </c>
       <c r="BD98" s="26"/>
       <c r="BE98" s="27"/>
-      <c r="BF98" s="81"/>
+      <c r="BF98" s="56"/>
       <c r="BG98" s="26"/>
       <c r="BH98" s="26"/>
       <c r="BI98" s="26"/>
@@ -11405,7 +11405,7 @@
       <c r="BV98" s="26"/>
       <c r="BW98" s="26"/>
       <c r="BX98" s="26"/>
-      <c r="BY98" s="83"/>
+      <c r="BY98" s="58"/>
     </row>
     <row r="99" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
@@ -11488,7 +11488,7 @@
         <v>2</v>
       </c>
       <c r="BE99" s="27"/>
-      <c r="BF99" s="81"/>
+      <c r="BF99" s="56"/>
       <c r="BG99" s="26"/>
       <c r="BH99" s="26"/>
       <c r="BI99" s="26"/>
@@ -11507,7 +11507,7 @@
       <c r="BV99" s="26"/>
       <c r="BW99" s="26"/>
       <c r="BX99" s="26"/>
-      <c r="BY99" s="83"/>
+      <c r="BY99" s="58"/>
     </row>
     <row r="100" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
@@ -11592,7 +11592,7 @@
       <c r="BE100" s="38">
         <v>5</v>
       </c>
-      <c r="BF100" s="81"/>
+      <c r="BF100" s="56"/>
       <c r="BG100" s="26"/>
       <c r="BH100" s="26"/>
       <c r="BI100" s="26"/>
@@ -11611,7 +11611,7 @@
       <c r="BV100" s="26"/>
       <c r="BW100" s="26"/>
       <c r="BX100" s="26"/>
-      <c r="BY100" s="83"/>
+      <c r="BY100" s="58"/>
     </row>
     <row r="101" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
@@ -11694,7 +11694,7 @@
       <c r="BE101" s="38">
         <v>2</v>
       </c>
-      <c r="BF101" s="81"/>
+      <c r="BF101" s="56"/>
       <c r="BG101" s="26"/>
       <c r="BH101" s="26"/>
       <c r="BI101" s="26"/>
@@ -11713,7 +11713,7 @@
       <c r="BV101" s="26"/>
       <c r="BW101" s="26"/>
       <c r="BX101" s="26"/>
-      <c r="BY101" s="83"/>
+      <c r="BY101" s="58"/>
     </row>
     <row r="102" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
@@ -11794,7 +11794,7 @@
       <c r="BC102" s="26"/>
       <c r="BD102" s="26"/>
       <c r="BE102" s="27"/>
-      <c r="BF102" s="81"/>
+      <c r="BF102" s="56"/>
       <c r="BG102" s="34">
         <v>1</v>
       </c>
@@ -11815,7 +11815,7 @@
       <c r="BV102" s="26"/>
       <c r="BW102" s="26"/>
       <c r="BX102" s="26"/>
-      <c r="BY102" s="83"/>
+      <c r="BY102" s="58"/>
     </row>
     <row r="103" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
@@ -11896,7 +11896,7 @@
       <c r="BC103" s="26"/>
       <c r="BD103" s="26"/>
       <c r="BE103" s="27"/>
-      <c r="BF103" s="81"/>
+      <c r="BF103" s="56"/>
       <c r="BG103" s="34">
         <v>2</v>
       </c>
@@ -11917,7 +11917,7 @@
       <c r="BV103" s="26"/>
       <c r="BW103" s="26"/>
       <c r="BX103" s="26"/>
-      <c r="BY103" s="83"/>
+      <c r="BY103" s="58"/>
     </row>
     <row r="104" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
@@ -11979,7 +11979,7 @@
       <c r="BC104" s="26"/>
       <c r="BD104" s="26"/>
       <c r="BE104" s="27"/>
-      <c r="BF104" s="81"/>
+      <c r="BF104" s="56"/>
       <c r="BG104" s="26"/>
       <c r="BH104" s="26"/>
       <c r="BI104" s="26"/>
@@ -11998,7 +11998,7 @@
       <c r="BV104" s="26"/>
       <c r="BW104" s="26"/>
       <c r="BX104" s="26"/>
-      <c r="BY104" s="83"/>
+      <c r="BY104" s="58"/>
     </row>
     <row r="105" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
@@ -12071,7 +12071,7 @@
       <c r="BC105" s="26"/>
       <c r="BD105" s="26"/>
       <c r="BE105" s="27"/>
-      <c r="BF105" s="81"/>
+      <c r="BF105" s="56"/>
       <c r="BG105" s="26"/>
       <c r="BH105" s="26"/>
       <c r="BI105" s="26"/>
@@ -12090,7 +12090,7 @@
       <c r="BV105" s="26"/>
       <c r="BW105" s="26"/>
       <c r="BX105" s="26"/>
-      <c r="BY105" s="83"/>
+      <c r="BY105" s="58"/>
     </row>
     <row r="106" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -12173,7 +12173,7 @@
       <c r="BC106" s="26"/>
       <c r="BD106" s="26"/>
       <c r="BE106" s="27"/>
-      <c r="BF106" s="81"/>
+      <c r="BF106" s="56"/>
       <c r="BG106" s="26"/>
       <c r="BH106" s="26"/>
       <c r="BI106" s="26"/>
@@ -12192,7 +12192,7 @@
       <c r="BV106" s="26"/>
       <c r="BW106" s="26"/>
       <c r="BX106" s="26"/>
-      <c r="BY106" s="83"/>
+      <c r="BY106" s="58"/>
     </row>
     <row r="107" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
@@ -12269,7 +12269,7 @@
       <c r="BC107" s="26"/>
       <c r="BD107" s="26"/>
       <c r="BE107" s="27"/>
-      <c r="BF107" s="81"/>
+      <c r="BF107" s="56"/>
       <c r="BG107" s="26"/>
       <c r="BH107" s="26"/>
       <c r="BI107" s="26"/>
@@ -12288,7 +12288,7 @@
       <c r="BV107" s="26"/>
       <c r="BW107" s="26"/>
       <c r="BX107" s="26"/>
-      <c r="BY107" s="83"/>
+      <c r="BY107" s="58"/>
     </row>
     <row r="108" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
@@ -12365,7 +12365,7 @@
       <c r="BC108" s="26"/>
       <c r="BD108" s="26"/>
       <c r="BE108" s="27"/>
-      <c r="BF108" s="81"/>
+      <c r="BF108" s="56"/>
       <c r="BG108" s="26"/>
       <c r="BH108" s="26"/>
       <c r="BI108" s="26"/>
@@ -12384,7 +12384,7 @@
       <c r="BV108" s="26"/>
       <c r="BW108" s="26"/>
       <c r="BX108" s="26"/>
-      <c r="BY108" s="83"/>
+      <c r="BY108" s="58"/>
     </row>
     <row r="109" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
@@ -12465,7 +12465,7 @@
       <c r="BC109" s="26"/>
       <c r="BD109" s="26"/>
       <c r="BE109" s="27"/>
-      <c r="BF109" s="81"/>
+      <c r="BF109" s="56"/>
       <c r="BG109" s="34">
         <v>4</v>
       </c>
@@ -12488,7 +12488,7 @@
       <c r="BV109" s="26"/>
       <c r="BW109" s="26"/>
       <c r="BX109" s="26"/>
-      <c r="BY109" s="83"/>
+      <c r="BY109" s="58"/>
     </row>
     <row r="110" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
@@ -12569,7 +12569,7 @@
       <c r="BC110" s="26"/>
       <c r="BD110" s="26"/>
       <c r="BE110" s="27"/>
-      <c r="BF110" s="81"/>
+      <c r="BF110" s="56"/>
       <c r="BG110" s="26"/>
       <c r="BH110" s="34">
         <v>2</v>
@@ -12590,7 +12590,7 @@
       <c r="BV110" s="26"/>
       <c r="BW110" s="26"/>
       <c r="BX110" s="26"/>
-      <c r="BY110" s="83"/>
+      <c r="BY110" s="58"/>
     </row>
     <row r="111" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
@@ -12671,7 +12671,7 @@
       <c r="BC111" s="26"/>
       <c r="BD111" s="26"/>
       <c r="BE111" s="27"/>
-      <c r="BF111" s="81"/>
+      <c r="BF111" s="56"/>
       <c r="BG111" s="26"/>
       <c r="BH111" s="26"/>
       <c r="BI111" s="34">
@@ -12692,7 +12692,7 @@
       <c r="BV111" s="26"/>
       <c r="BW111" s="26"/>
       <c r="BX111" s="26"/>
-      <c r="BY111" s="83"/>
+      <c r="BY111" s="58"/>
     </row>
     <row r="112" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
@@ -12773,7 +12773,7 @@
       <c r="BC112" s="26"/>
       <c r="BD112" s="26"/>
       <c r="BE112" s="27"/>
-      <c r="BF112" s="81"/>
+      <c r="BF112" s="56"/>
       <c r="BG112" s="26"/>
       <c r="BH112" s="26"/>
       <c r="BI112" s="34">
@@ -12794,7 +12794,7 @@
       <c r="BV112" s="26"/>
       <c r="BW112" s="26"/>
       <c r="BX112" s="26"/>
-      <c r="BY112" s="83"/>
+      <c r="BY112" s="58"/>
     </row>
     <row r="113" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
@@ -12865,7 +12865,7 @@
       <c r="BC113" s="26"/>
       <c r="BD113" s="26"/>
       <c r="BE113" s="27"/>
-      <c r="BF113" s="81"/>
+      <c r="BF113" s="56"/>
       <c r="BG113" s="26"/>
       <c r="BH113" s="26"/>
       <c r="BI113" s="26"/>
@@ -12884,7 +12884,7 @@
       <c r="BV113" s="26"/>
       <c r="BW113" s="26"/>
       <c r="BX113" s="26"/>
-      <c r="BY113" s="83"/>
+      <c r="BY113" s="58"/>
     </row>
     <row r="114" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
@@ -12957,7 +12957,7 @@
       <c r="BC114" s="26"/>
       <c r="BD114" s="26"/>
       <c r="BE114" s="27"/>
-      <c r="BF114" s="81"/>
+      <c r="BF114" s="56"/>
       <c r="BG114" s="26"/>
       <c r="BH114" s="26"/>
       <c r="BI114" s="26"/>
@@ -12976,7 +12976,7 @@
       <c r="BV114" s="26"/>
       <c r="BW114" s="26"/>
       <c r="BX114" s="26"/>
-      <c r="BY114" s="83"/>
+      <c r="BY114" s="58"/>
     </row>
     <row r="115" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
@@ -13063,7 +13063,7 @@
       <c r="BC115" s="26"/>
       <c r="BD115" s="26"/>
       <c r="BE115" s="27"/>
-      <c r="BF115" s="81"/>
+      <c r="BF115" s="56"/>
       <c r="BG115" s="26"/>
       <c r="BH115" s="26"/>
       <c r="BI115" s="26"/>
@@ -13082,7 +13082,7 @@
       <c r="BV115" s="26"/>
       <c r="BW115" s="26"/>
       <c r="BX115" s="26"/>
-      <c r="BY115" s="83"/>
+      <c r="BY115" s="58"/>
     </row>
     <row r="116" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
@@ -13159,7 +13159,7 @@
       <c r="BC116" s="26"/>
       <c r="BD116" s="26"/>
       <c r="BE116" s="27"/>
-      <c r="BF116" s="81"/>
+      <c r="BF116" s="56"/>
       <c r="BG116" s="26"/>
       <c r="BH116" s="26"/>
       <c r="BI116" s="26"/>
@@ -13178,7 +13178,7 @@
       <c r="BV116" s="26"/>
       <c r="BW116" s="26"/>
       <c r="BX116" s="26"/>
-      <c r="BY116" s="83"/>
+      <c r="BY116" s="58"/>
     </row>
     <row r="117" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
@@ -13255,7 +13255,7 @@
       <c r="BC117" s="26"/>
       <c r="BD117" s="26"/>
       <c r="BE117" s="27"/>
-      <c r="BF117" s="81"/>
+      <c r="BF117" s="56"/>
       <c r="BG117" s="26"/>
       <c r="BH117" s="26"/>
       <c r="BI117" s="26"/>
@@ -13274,7 +13274,7 @@
       <c r="BV117" s="26"/>
       <c r="BW117" s="26"/>
       <c r="BX117" s="26"/>
-      <c r="BY117" s="83"/>
+      <c r="BY117" s="58"/>
     </row>
     <row r="118" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
@@ -13365,7 +13365,7 @@
       <c r="BC118" s="26"/>
       <c r="BD118" s="26"/>
       <c r="BE118" s="27"/>
-      <c r="BF118" s="81"/>
+      <c r="BF118" s="56"/>
       <c r="BG118" s="26"/>
       <c r="BH118" s="26"/>
       <c r="BI118" s="26"/>
@@ -13384,7 +13384,7 @@
       <c r="BV118" s="26"/>
       <c r="BW118" s="26"/>
       <c r="BX118" s="26"/>
-      <c r="BY118" s="83"/>
+      <c r="BY118" s="58"/>
     </row>
     <row r="119" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
@@ -13461,7 +13461,7 @@
       <c r="BC119" s="26"/>
       <c r="BD119" s="26"/>
       <c r="BE119" s="27"/>
-      <c r="BF119" s="81"/>
+      <c r="BF119" s="56"/>
       <c r="BG119" s="26"/>
       <c r="BH119" s="26"/>
       <c r="BI119" s="26"/>
@@ -13480,7 +13480,7 @@
       <c r="BV119" s="26"/>
       <c r="BW119" s="26"/>
       <c r="BX119" s="26"/>
-      <c r="BY119" s="83"/>
+      <c r="BY119" s="58"/>
     </row>
     <row r="120" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
@@ -13556,7 +13556,7 @@
       <c r="BC120" s="26"/>
       <c r="BD120" s="26"/>
       <c r="BE120" s="27"/>
-      <c r="BF120" s="81"/>
+      <c r="BF120" s="56"/>
       <c r="BG120" s="26"/>
       <c r="BH120" s="26"/>
       <c r="BI120" s="26"/>
@@ -13575,7 +13575,7 @@
       <c r="BV120" s="26"/>
       <c r="BW120" s="26"/>
       <c r="BX120" s="26"/>
-      <c r="BY120" s="83"/>
+      <c r="BY120" s="58"/>
     </row>
     <row r="121" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
@@ -13658,7 +13658,7 @@
       <c r="BC121" s="26"/>
       <c r="BD121" s="26"/>
       <c r="BE121" s="27"/>
-      <c r="BF121" s="81"/>
+      <c r="BF121" s="56"/>
       <c r="BG121" s="26"/>
       <c r="BH121" s="26"/>
       <c r="BI121" s="26"/>
@@ -13677,7 +13677,7 @@
       <c r="BV121" s="26"/>
       <c r="BW121" s="26"/>
       <c r="BX121" s="26"/>
-      <c r="BY121" s="83"/>
+      <c r="BY121" s="58"/>
     </row>
     <row r="122" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -13748,7 +13748,7 @@
       <c r="BC122" s="26"/>
       <c r="BD122" s="26"/>
       <c r="BE122" s="27"/>
-      <c r="BF122" s="81"/>
+      <c r="BF122" s="56"/>
       <c r="BG122" s="26"/>
       <c r="BH122" s="26"/>
       <c r="BI122" s="26"/>
@@ -13767,7 +13767,7 @@
       <c r="BV122" s="26"/>
       <c r="BW122" s="26"/>
       <c r="BX122" s="26"/>
-      <c r="BY122" s="83"/>
+      <c r="BY122" s="58"/>
     </row>
     <row r="123" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
@@ -13840,7 +13840,7 @@
       <c r="BC123" s="26"/>
       <c r="BD123" s="26"/>
       <c r="BE123" s="27"/>
-      <c r="BF123" s="81"/>
+      <c r="BF123" s="56"/>
       <c r="BG123" s="26"/>
       <c r="BH123" s="26"/>
       <c r="BI123" s="26"/>
@@ -13859,7 +13859,7 @@
       <c r="BV123" s="26"/>
       <c r="BW123" s="26"/>
       <c r="BX123" s="26"/>
-      <c r="BY123" s="83"/>
+      <c r="BY123" s="58"/>
     </row>
     <row r="124" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
@@ -13948,7 +13948,7 @@
       <c r="BC124" s="26"/>
       <c r="BD124" s="26"/>
       <c r="BE124" s="27"/>
-      <c r="BF124" s="81"/>
+      <c r="BF124" s="56"/>
       <c r="BG124" s="26"/>
       <c r="BH124" s="26"/>
       <c r="BI124" s="26"/>
@@ -13967,7 +13967,7 @@
       <c r="BV124" s="26"/>
       <c r="BW124" s="26"/>
       <c r="BX124" s="26"/>
-      <c r="BY124" s="83"/>
+      <c r="BY124" s="58"/>
     </row>
     <row r="125" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
@@ -14054,7 +14054,7 @@
       <c r="BC125" s="26"/>
       <c r="BD125" s="26"/>
       <c r="BE125" s="27"/>
-      <c r="BF125" s="81"/>
+      <c r="BF125" s="56"/>
       <c r="BG125" s="26"/>
       <c r="BH125" s="26"/>
       <c r="BI125" s="26"/>
@@ -14073,7 +14073,7 @@
       <c r="BV125" s="26"/>
       <c r="BW125" s="26"/>
       <c r="BX125" s="26"/>
-      <c r="BY125" s="83"/>
+      <c r="BY125" s="58"/>
     </row>
     <row r="126" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
@@ -14158,7 +14158,7 @@
       <c r="BC126" s="26"/>
       <c r="BD126" s="26"/>
       <c r="BE126" s="27"/>
-      <c r="BF126" s="81"/>
+      <c r="BF126" s="56"/>
       <c r="BG126" s="26"/>
       <c r="BH126" s="26"/>
       <c r="BI126" s="26"/>
@@ -14177,7 +14177,7 @@
       <c r="BV126" s="26"/>
       <c r="BW126" s="26"/>
       <c r="BX126" s="26"/>
-      <c r="BY126" s="83"/>
+      <c r="BY126" s="58"/>
     </row>
     <row r="127" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
@@ -14264,7 +14264,7 @@
       <c r="BC127" s="26"/>
       <c r="BD127" s="26"/>
       <c r="BE127" s="27"/>
-      <c r="BF127" s="81"/>
+      <c r="BF127" s="56"/>
       <c r="BG127" s="26"/>
       <c r="BH127" s="26"/>
       <c r="BI127" s="26"/>
@@ -14283,7 +14283,7 @@
       <c r="BV127" s="26"/>
       <c r="BW127" s="26"/>
       <c r="BX127" s="26"/>
-      <c r="BY127" s="83"/>
+      <c r="BY127" s="58"/>
     </row>
     <row r="128" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
@@ -14364,7 +14364,7 @@
       <c r="BC128" s="26"/>
       <c r="BD128" s="26"/>
       <c r="BE128" s="27"/>
-      <c r="BF128" s="81"/>
+      <c r="BF128" s="56"/>
       <c r="BG128" s="26"/>
       <c r="BH128" s="26"/>
       <c r="BI128" s="26"/>
@@ -14393,7 +14393,7 @@
       <c r="BV128" s="26"/>
       <c r="BW128" s="26"/>
       <c r="BX128" s="26"/>
-      <c r="BY128" s="83"/>
+      <c r="BY128" s="58"/>
     </row>
     <row r="129" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
@@ -14474,7 +14474,7 @@
       <c r="BC129" s="26"/>
       <c r="BD129" s="26"/>
       <c r="BE129" s="27"/>
-      <c r="BF129" s="81"/>
+      <c r="BF129" s="56"/>
       <c r="BG129" s="26"/>
       <c r="BH129" s="26"/>
       <c r="BI129" s="26"/>
@@ -14499,7 +14499,7 @@
       <c r="BV129" s="26"/>
       <c r="BW129" s="26"/>
       <c r="BX129" s="26"/>
-      <c r="BY129" s="83"/>
+      <c r="BY129" s="58"/>
     </row>
     <row r="130" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
@@ -14580,7 +14580,7 @@
       <c r="BC130" s="26"/>
       <c r="BD130" s="26"/>
       <c r="BE130" s="27"/>
-      <c r="BF130" s="81"/>
+      <c r="BF130" s="56"/>
       <c r="BG130" s="26"/>
       <c r="BH130" s="26"/>
       <c r="BI130" s="26"/>
@@ -14605,7 +14605,7 @@
       <c r="BV130" s="26"/>
       <c r="BW130" s="26"/>
       <c r="BX130" s="26"/>
-      <c r="BY130" s="83"/>
+      <c r="BY130" s="58"/>
     </row>
     <row r="131" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
@@ -14686,7 +14686,7 @@
       <c r="BC131" s="26"/>
       <c r="BD131" s="26"/>
       <c r="BE131" s="27"/>
-      <c r="BF131" s="81"/>
+      <c r="BF131" s="56"/>
       <c r="BG131" s="26"/>
       <c r="BH131" s="26"/>
       <c r="BI131" s="34">
@@ -14709,7 +14709,7 @@
       <c r="BV131" s="26"/>
       <c r="BW131" s="26"/>
       <c r="BX131" s="26"/>
-      <c r="BY131" s="83"/>
+      <c r="BY131" s="58"/>
     </row>
     <row r="132" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
@@ -14788,7 +14788,7 @@
       <c r="BC132" s="26"/>
       <c r="BD132" s="26"/>
       <c r="BE132" s="27"/>
-      <c r="BF132" s="81"/>
+      <c r="BF132" s="56"/>
       <c r="BG132" s="26"/>
       <c r="BH132" s="26"/>
       <c r="BI132" s="26"/>
@@ -14811,7 +14811,7 @@
       <c r="BV132" s="26"/>
       <c r="BW132" s="26"/>
       <c r="BX132" s="26"/>
-      <c r="BY132" s="83"/>
+      <c r="BY132" s="58"/>
     </row>
     <row r="133" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
@@ -14882,7 +14882,7 @@
       <c r="BC133" s="26"/>
       <c r="BD133" s="26"/>
       <c r="BE133" s="27"/>
-      <c r="BF133" s="81"/>
+      <c r="BF133" s="56"/>
       <c r="BG133" s="26"/>
       <c r="BH133" s="26"/>
       <c r="BI133" s="26"/>
@@ -14901,7 +14901,7 @@
       <c r="BV133" s="26"/>
       <c r="BW133" s="26"/>
       <c r="BX133" s="26"/>
-      <c r="BY133" s="83"/>
+      <c r="BY133" s="58"/>
     </row>
     <row r="134" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
@@ -14974,7 +14974,7 @@
       <c r="BC134" s="26"/>
       <c r="BD134" s="26"/>
       <c r="BE134" s="27"/>
-      <c r="BF134" s="81"/>
+      <c r="BF134" s="56"/>
       <c r="BG134" s="26"/>
       <c r="BH134" s="26"/>
       <c r="BI134" s="26"/>
@@ -14993,7 +14993,7 @@
       <c r="BV134" s="26"/>
       <c r="BW134" s="26"/>
       <c r="BX134" s="26"/>
-      <c r="BY134" s="83"/>
+      <c r="BY134" s="58"/>
     </row>
     <row r="135" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
@@ -15162,7 +15162,7 @@
       <c r="BE135" s="38">
         <v>1</v>
       </c>
-      <c r="BF135" s="81"/>
+      <c r="BF135" s="56"/>
       <c r="BG135" s="38">
         <v>1</v>
       </c>
@@ -15290,7 +15290,7 @@
       <c r="BC136" s="26"/>
       <c r="BD136" s="26"/>
       <c r="BE136" s="27"/>
-      <c r="BF136" s="81"/>
+      <c r="BF136" s="56"/>
       <c r="BG136" s="26"/>
       <c r="BH136" s="26"/>
       <c r="BI136" s="26"/>
@@ -15309,13 +15309,13 @@
       <c r="BV136" s="26"/>
       <c r="BW136" s="26"/>
       <c r="BX136" s="26"/>
-      <c r="BY136" s="83"/>
+      <c r="BY136" s="58"/>
     </row>
     <row r="137" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>129</v>
       </c>
-      <c r="B137" s="64" t="s">
+      <c r="B137" s="40" t="s">
         <v>89</v>
       </c>
       <c r="C137" s="3"/>
@@ -15337,97 +15337,97 @@
       <c r="J137" s="32"/>
       <c r="K137" s="32"/>
       <c r="L137" s="2"/>
-      <c r="M137" s="71"/>
-      <c r="N137" s="72"/>
-      <c r="O137" s="72"/>
-      <c r="P137" s="72"/>
-      <c r="Q137" s="73"/>
-      <c r="R137" s="71"/>
-      <c r="S137" s="72"/>
-      <c r="T137" s="72"/>
-      <c r="U137" s="72"/>
-      <c r="V137" s="73"/>
-      <c r="W137" s="71">
+      <c r="M137" s="47"/>
+      <c r="N137" s="48"/>
+      <c r="O137" s="48"/>
+      <c r="P137" s="48"/>
+      <c r="Q137" s="49"/>
+      <c r="R137" s="47"/>
+      <c r="S137" s="48"/>
+      <c r="T137" s="48"/>
+      <c r="U137" s="48"/>
+      <c r="V137" s="49"/>
+      <c r="W137" s="47">
         <v>3</v>
       </c>
-      <c r="X137" s="72">
+      <c r="X137" s="48">
         <v>3</v>
       </c>
-      <c r="Y137" s="72">
+      <c r="Y137" s="48">
         <v>3</v>
       </c>
-      <c r="Z137" s="72">
+      <c r="Z137" s="48">
         <v>3</v>
       </c>
-      <c r="AA137" s="73">
+      <c r="AA137" s="49">
         <v>3</v>
       </c>
-      <c r="AB137" s="71">
+      <c r="AB137" s="47">
         <v>3</v>
       </c>
-      <c r="AC137" s="72">
+      <c r="AC137" s="48">
         <v>3</v>
       </c>
-      <c r="AD137" s="72">
+      <c r="AD137" s="48">
         <v>3</v>
       </c>
-      <c r="AE137" s="72">
+      <c r="AE137" s="48">
         <v>3</v>
       </c>
-      <c r="AF137" s="72">
+      <c r="AF137" s="48">
         <v>3</v>
       </c>
-      <c r="AG137" s="71"/>
-      <c r="AH137" s="72"/>
-      <c r="AI137" s="72"/>
-      <c r="AJ137" s="72"/>
-      <c r="AK137" s="73"/>
-      <c r="AL137" s="71"/>
-      <c r="AM137" s="72"/>
-      <c r="AN137" s="72"/>
-      <c r="AO137" s="72"/>
-      <c r="AP137" s="73"/>
-      <c r="AQ137" s="71"/>
-      <c r="AR137" s="72"/>
-      <c r="AS137" s="72"/>
-      <c r="AT137" s="72"/>
-      <c r="AU137" s="72"/>
-      <c r="AV137" s="71"/>
-      <c r="AW137" s="72"/>
-      <c r="AX137" s="72"/>
-      <c r="AY137" s="72"/>
-      <c r="AZ137" s="72"/>
-      <c r="BA137" s="71"/>
-      <c r="BB137" s="72"/>
-      <c r="BC137" s="72"/>
-      <c r="BD137" s="72"/>
-      <c r="BE137" s="73"/>
-      <c r="BF137" s="81"/>
-      <c r="BG137" s="72"/>
-      <c r="BH137" s="72"/>
-      <c r="BI137" s="72"/>
-      <c r="BJ137" s="72"/>
-      <c r="BK137" s="71"/>
-      <c r="BL137" s="72"/>
-      <c r="BM137" s="72"/>
-      <c r="BN137" s="72"/>
-      <c r="BO137" s="72"/>
-      <c r="BP137" s="71"/>
-      <c r="BQ137" s="72"/>
-      <c r="BR137" s="72"/>
-      <c r="BS137" s="72"/>
-      <c r="BT137" s="72"/>
-      <c r="BU137" s="71"/>
-      <c r="BV137" s="72"/>
-      <c r="BW137" s="72"/>
-      <c r="BX137" s="72"/>
-      <c r="BY137" s="73"/>
+      <c r="AG137" s="47"/>
+      <c r="AH137" s="48"/>
+      <c r="AI137" s="48"/>
+      <c r="AJ137" s="48"/>
+      <c r="AK137" s="49"/>
+      <c r="AL137" s="47"/>
+      <c r="AM137" s="48"/>
+      <c r="AN137" s="48"/>
+      <c r="AO137" s="48"/>
+      <c r="AP137" s="49"/>
+      <c r="AQ137" s="47"/>
+      <c r="AR137" s="48"/>
+      <c r="AS137" s="48"/>
+      <c r="AT137" s="48"/>
+      <c r="AU137" s="48"/>
+      <c r="AV137" s="47"/>
+      <c r="AW137" s="48"/>
+      <c r="AX137" s="48"/>
+      <c r="AY137" s="48"/>
+      <c r="AZ137" s="48"/>
+      <c r="BA137" s="47"/>
+      <c r="BB137" s="48"/>
+      <c r="BC137" s="48"/>
+      <c r="BD137" s="48"/>
+      <c r="BE137" s="49"/>
+      <c r="BF137" s="56"/>
+      <c r="BG137" s="48"/>
+      <c r="BH137" s="48"/>
+      <c r="BI137" s="48"/>
+      <c r="BJ137" s="48"/>
+      <c r="BK137" s="47"/>
+      <c r="BL137" s="48"/>
+      <c r="BM137" s="48"/>
+      <c r="BN137" s="48"/>
+      <c r="BO137" s="48"/>
+      <c r="BP137" s="47"/>
+      <c r="BQ137" s="48"/>
+      <c r="BR137" s="48"/>
+      <c r="BS137" s="48"/>
+      <c r="BT137" s="48"/>
+      <c r="BU137" s="47"/>
+      <c r="BV137" s="48"/>
+      <c r="BW137" s="48"/>
+      <c r="BX137" s="48"/>
+      <c r="BY137" s="49"/>
     </row>
     <row r="138" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>130</v>
       </c>
-      <c r="B138" s="64"/>
+      <c r="B138" s="40"/>
       <c r="C138" s="3"/>
       <c r="D138" s="4">
         <f t="shared" si="0"/>
@@ -15486,7 +15486,7 @@
       <c r="BC138" s="26"/>
       <c r="BD138" s="26"/>
       <c r="BE138" s="27"/>
-      <c r="BF138" s="81"/>
+      <c r="BF138" s="56"/>
       <c r="BG138" s="26"/>
       <c r="BH138" s="26"/>
       <c r="BI138" s="26"/>
@@ -15505,7 +15505,7 @@
       <c r="BV138" s="26"/>
       <c r="BW138" s="26"/>
       <c r="BX138" s="26"/>
-      <c r="BY138" s="83"/>
+      <c r="BY138" s="58"/>
     </row>
     <row r="139" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
@@ -15531,93 +15531,93 @@
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
       <c r="L139" s="2"/>
-      <c r="M139" s="65"/>
-      <c r="N139" s="66"/>
-      <c r="O139" s="66"/>
-      <c r="P139" s="66"/>
-      <c r="Q139" s="67"/>
-      <c r="R139" s="65"/>
-      <c r="S139" s="66"/>
-      <c r="T139" s="66"/>
-      <c r="U139" s="66"/>
-      <c r="V139" s="68"/>
-      <c r="W139" s="65"/>
-      <c r="X139" s="66"/>
-      <c r="Y139" s="66"/>
-      <c r="Z139" s="66"/>
-      <c r="AA139" s="68"/>
-      <c r="AB139" s="69"/>
-      <c r="AC139" s="70"/>
-      <c r="AD139" s="70"/>
-      <c r="AE139" s="70"/>
-      <c r="AF139" s="70"/>
-      <c r="AG139" s="69"/>
-      <c r="AH139" s="70"/>
-      <c r="AI139" s="70"/>
-      <c r="AJ139" s="70"/>
-      <c r="AK139" s="68"/>
-      <c r="AL139" s="65"/>
-      <c r="AM139" s="66"/>
-      <c r="AN139" s="66"/>
-      <c r="AO139" s="66"/>
-      <c r="AP139" s="68"/>
-      <c r="AQ139" s="65"/>
-      <c r="AR139" s="66"/>
-      <c r="AS139" s="66"/>
-      <c r="AT139" s="66"/>
-      <c r="AU139" s="66"/>
-      <c r="AV139" s="65"/>
-      <c r="AW139" s="66"/>
-      <c r="AX139" s="66"/>
-      <c r="AY139" s="66"/>
-      <c r="AZ139" s="66"/>
-      <c r="BA139" s="65"/>
-      <c r="BB139" s="66"/>
-      <c r="BC139" s="66"/>
-      <c r="BD139" s="66"/>
-      <c r="BE139" s="68"/>
-      <c r="BF139" s="81"/>
-      <c r="BG139" s="66"/>
-      <c r="BH139" s="66"/>
-      <c r="BI139" s="66"/>
-      <c r="BJ139" s="66"/>
-      <c r="BK139" s="65"/>
-      <c r="BL139" s="66"/>
-      <c r="BM139" s="66"/>
-      <c r="BN139" s="66"/>
-      <c r="BO139" s="66"/>
-      <c r="BP139" s="65"/>
-      <c r="BQ139" s="66"/>
-      <c r="BR139" s="66"/>
-      <c r="BS139" s="66"/>
-      <c r="BT139" s="66"/>
-      <c r="BU139" s="65"/>
-      <c r="BV139" s="66"/>
-      <c r="BW139" s="66"/>
-      <c r="BX139" s="66"/>
-      <c r="BY139" s="83"/>
+      <c r="M139" s="41"/>
+      <c r="N139" s="42"/>
+      <c r="O139" s="42"/>
+      <c r="P139" s="42"/>
+      <c r="Q139" s="43"/>
+      <c r="R139" s="41"/>
+      <c r="S139" s="42"/>
+      <c r="T139" s="42"/>
+      <c r="U139" s="42"/>
+      <c r="V139" s="44"/>
+      <c r="W139" s="41"/>
+      <c r="X139" s="42"/>
+      <c r="Y139" s="42"/>
+      <c r="Z139" s="42"/>
+      <c r="AA139" s="44"/>
+      <c r="AB139" s="45"/>
+      <c r="AC139" s="46"/>
+      <c r="AD139" s="46"/>
+      <c r="AE139" s="46"/>
+      <c r="AF139" s="46"/>
+      <c r="AG139" s="45"/>
+      <c r="AH139" s="46"/>
+      <c r="AI139" s="46"/>
+      <c r="AJ139" s="46"/>
+      <c r="AK139" s="44"/>
+      <c r="AL139" s="41"/>
+      <c r="AM139" s="42"/>
+      <c r="AN139" s="42"/>
+      <c r="AO139" s="42"/>
+      <c r="AP139" s="44"/>
+      <c r="AQ139" s="41"/>
+      <c r="AR139" s="42"/>
+      <c r="AS139" s="42"/>
+      <c r="AT139" s="42"/>
+      <c r="AU139" s="42"/>
+      <c r="AV139" s="41"/>
+      <c r="AW139" s="42"/>
+      <c r="AX139" s="42"/>
+      <c r="AY139" s="42"/>
+      <c r="AZ139" s="42"/>
+      <c r="BA139" s="41"/>
+      <c r="BB139" s="42"/>
+      <c r="BC139" s="42"/>
+      <c r="BD139" s="42"/>
+      <c r="BE139" s="44"/>
+      <c r="BF139" s="56"/>
+      <c r="BG139" s="42"/>
+      <c r="BH139" s="42"/>
+      <c r="BI139" s="42"/>
+      <c r="BJ139" s="42"/>
+      <c r="BK139" s="41"/>
+      <c r="BL139" s="42"/>
+      <c r="BM139" s="42"/>
+      <c r="BN139" s="42"/>
+      <c r="BO139" s="42"/>
+      <c r="BP139" s="41"/>
+      <c r="BQ139" s="42"/>
+      <c r="BR139" s="42"/>
+      <c r="BS139" s="42"/>
+      <c r="BT139" s="42"/>
+      <c r="BU139" s="41"/>
+      <c r="BV139" s="42"/>
+      <c r="BW139" s="42"/>
+      <c r="BX139" s="42"/>
+      <c r="BY139" s="58"/>
     </row>
     <row r="140" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A140" s="46" t="s">
+      <c r="A140" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="B140" s="47"/>
-      <c r="C140" s="47"/>
-      <c r="D140" s="47"/>
-      <c r="E140" s="47"/>
-      <c r="F140" s="47"/>
-      <c r="G140" s="47"/>
-      <c r="H140" s="47"/>
-      <c r="I140" s="47"/>
-      <c r="J140" s="47"/>
-      <c r="K140" s="47"/>
-      <c r="L140" s="48"/>
+      <c r="B140" s="76"/>
+      <c r="C140" s="76"/>
+      <c r="D140" s="76"/>
+      <c r="E140" s="76"/>
+      <c r="F140" s="76"/>
+      <c r="G140" s="76"/>
+      <c r="H140" s="76"/>
+      <c r="I140" s="76"/>
+      <c r="J140" s="76"/>
+      <c r="K140" s="76"/>
+      <c r="L140" s="77"/>
       <c r="M140" s="31">
         <f>SUM(M10:M139)</f>
         <v>0</v>
       </c>
       <c r="N140" s="31">
-        <f t="shared" ref="N140:AG140" si="16">SUM(N10:N139)</f>
+        <f t="shared" ref="N140:AE140" si="16">SUM(N10:N139)</f>
         <v>8</v>
       </c>
       <c r="O140" s="31">
@@ -15708,7 +15708,7 @@
         <f t="shared" ref="AJ140" si="21">SUM(AJ10:AJ139)</f>
         <v>8</v>
       </c>
-      <c r="AK140" s="76">
+      <c r="AK140" s="52">
         <f t="shared" ref="AK140" si="22">SUM(AK10:AK139)</f>
         <v>8</v>
       </c>
@@ -15716,19 +15716,19 @@
         <f t="shared" ref="AL140" si="23">SUM(AL10:AL139)</f>
         <v>8</v>
       </c>
-      <c r="AM140" s="74">
+      <c r="AM140" s="50">
         <f t="shared" ref="AM140" si="24">SUM(AM10:AM139)</f>
         <v>8</v>
       </c>
-      <c r="AN140" s="74">
+      <c r="AN140" s="50">
         <f t="shared" ref="AN140" si="25">SUM(AN10:AN139)</f>
         <v>8</v>
       </c>
-      <c r="AO140" s="74">
+      <c r="AO140" s="50">
         <f t="shared" ref="AO140" si="26">SUM(AO10:AO139)</f>
         <v>8</v>
       </c>
-      <c r="AP140" s="78">
+      <c r="AP140" s="53">
         <f t="shared" ref="AP140" si="27">SUM(AP10:AP139)</f>
         <v>8</v>
       </c>
@@ -15736,19 +15736,19 @@
         <f t="shared" ref="AQ140" si="28">SUM(AQ10:AQ139)</f>
         <v>8</v>
       </c>
-      <c r="AR140" s="74">
+      <c r="AR140" s="50">
         <f t="shared" ref="AR140" si="29">SUM(AR10:AR139)</f>
         <v>8</v>
       </c>
-      <c r="AS140" s="74">
+      <c r="AS140" s="50">
         <f t="shared" ref="AS140" si="30">SUM(AS10:AS139)</f>
         <v>8</v>
       </c>
-      <c r="AT140" s="74">
+      <c r="AT140" s="50">
         <f t="shared" ref="AT140" si="31">SUM(AT10:AT139)</f>
         <v>8</v>
       </c>
-      <c r="AU140" s="74">
+      <c r="AU140" s="50">
         <f t="shared" ref="AU140" si="32">SUM(AU10:AU139)</f>
         <v>8</v>
       </c>
@@ -15756,19 +15756,19 @@
         <f t="shared" ref="AV140" si="33">SUM(AV10:AV139)</f>
         <v>8</v>
       </c>
-      <c r="AW140" s="74">
+      <c r="AW140" s="50">
         <f t="shared" ref="AW140" si="34">SUM(AW10:AW139)</f>
         <v>8</v>
       </c>
-      <c r="AX140" s="74">
+      <c r="AX140" s="50">
         <f t="shared" ref="AX140" si="35">SUM(AX10:AX139)</f>
         <v>8</v>
       </c>
-      <c r="AY140" s="74">
+      <c r="AY140" s="50">
         <f t="shared" ref="AY140" si="36">SUM(AY10:AY139)</f>
         <v>8</v>
       </c>
-      <c r="AZ140" s="74">
+      <c r="AZ140" s="50">
         <f t="shared" ref="AZ140" si="37">SUM(AZ10:AZ139)</f>
         <v>8</v>
       </c>
@@ -15776,23 +15776,23 @@
         <f t="shared" ref="BA140" si="38">SUM(BA10:BA139)</f>
         <v>8</v>
       </c>
-      <c r="BB140" s="74">
+      <c r="BB140" s="50">
         <f t="shared" ref="BB140" si="39">SUM(BB10:BB139)</f>
         <v>8</v>
       </c>
-      <c r="BC140" s="74">
+      <c r="BC140" s="50">
         <f t="shared" ref="BC140" si="40">SUM(BC10:BC139)</f>
         <v>8</v>
       </c>
-      <c r="BD140" s="74">
+      <c r="BD140" s="50">
         <f t="shared" ref="BD140" si="41">SUM(BD10:BD139)</f>
         <v>8</v>
       </c>
-      <c r="BE140" s="78">
+      <c r="BE140" s="53">
         <f t="shared" ref="BE140" si="42">SUM(BE10:BE139)</f>
         <v>8</v>
       </c>
-      <c r="BF140" s="82">
+      <c r="BF140" s="57">
         <f t="shared" ref="BF140" si="43">SUM(BF10:BF139)</f>
         <v>0</v>
       </c>
@@ -15836,19 +15836,19 @@
         <f t="shared" ref="BP140" si="53">SUM(BP10:BP139)</f>
         <v>8</v>
       </c>
-      <c r="BQ140" s="74">
+      <c r="BQ140" s="50">
         <f t="shared" ref="BQ140" si="54">SUM(BQ10:BQ139)</f>
         <v>8</v>
       </c>
-      <c r="BR140" s="74">
+      <c r="BR140" s="50">
         <f t="shared" ref="BR140" si="55">SUM(BR10:BR139)</f>
         <v>8</v>
       </c>
-      <c r="BS140" s="74">
+      <c r="BS140" s="50">
         <f t="shared" ref="BS140" si="56">SUM(BS10:BS139)</f>
         <v>8</v>
       </c>
-      <c r="BT140" s="74">
+      <c r="BT140" s="50">
         <f t="shared" ref="BT140" si="57">SUM(BT10:BT139)</f>
         <v>8</v>
       </c>
@@ -15856,29 +15856,110 @@
         <f t="shared" ref="BU140" si="58">SUM(BU10:BU139)</f>
         <v>3</v>
       </c>
-      <c r="BV140" s="74">
+      <c r="BV140" s="50">
         <f t="shared" ref="BV140" si="59">SUM(BV10:BV139)</f>
         <v>1</v>
       </c>
-      <c r="BW140" s="74">
+      <c r="BW140" s="50">
         <f t="shared" ref="BW140" si="60">SUM(BW10:BW139)</f>
         <v>1</v>
       </c>
-      <c r="BX140" s="74">
+      <c r="BX140" s="50">
         <f t="shared" ref="BX140:BY140" si="61">SUM(BX10:BX139)</f>
         <v>1</v>
       </c>
-      <c r="BY140" s="78">
+      <c r="BY140" s="53">
         <f t="shared" si="61"/>
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:77" x14ac:dyDescent="0.25">
       <c r="BF141" s="29"/>
-      <c r="BG141" s="79"/>
+      <c r="BG141" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="97">
+    <mergeCell ref="BG4:BG6"/>
+    <mergeCell ref="BH4:BH6"/>
+    <mergeCell ref="BI4:BI6"/>
+    <mergeCell ref="BJ4:BJ6"/>
+    <mergeCell ref="BB4:BB6"/>
+    <mergeCell ref="BC4:BC6"/>
+    <mergeCell ref="BD4:BD6"/>
+    <mergeCell ref="BE4:BE6"/>
+    <mergeCell ref="BF4:BF6"/>
+    <mergeCell ref="AW4:AW6"/>
+    <mergeCell ref="AX4:AX6"/>
+    <mergeCell ref="AY4:AY6"/>
+    <mergeCell ref="AZ4:AZ6"/>
+    <mergeCell ref="BA4:BA6"/>
+    <mergeCell ref="AR4:AR6"/>
+    <mergeCell ref="AS4:AS6"/>
+    <mergeCell ref="AT4:AT6"/>
+    <mergeCell ref="AU4:AU6"/>
+    <mergeCell ref="AV4:AV6"/>
+    <mergeCell ref="AM4:AM6"/>
+    <mergeCell ref="AN4:AN6"/>
+    <mergeCell ref="AO4:AO6"/>
+    <mergeCell ref="AP4:AP6"/>
+    <mergeCell ref="AQ4:AQ6"/>
+    <mergeCell ref="AH4:AH6"/>
+    <mergeCell ref="AI4:AI6"/>
+    <mergeCell ref="AJ4:AJ6"/>
+    <mergeCell ref="AK4:AK6"/>
+    <mergeCell ref="AL4:AL6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AD4:AD6"/>
+    <mergeCell ref="AE4:AE6"/>
+    <mergeCell ref="AF4:AF6"/>
+    <mergeCell ref="AG4:AG6"/>
+    <mergeCell ref="X4:X6"/>
+    <mergeCell ref="Y4:Y6"/>
+    <mergeCell ref="Z4:Z6"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AB4:AB6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="U4:U6"/>
+    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A140:L140"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="BN4:BN6"/>
+    <mergeCell ref="BO4:BO6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="AL7:AP7"/>
+    <mergeCell ref="AQ7:AU7"/>
+    <mergeCell ref="AV7:AZ7"/>
+    <mergeCell ref="BA7:BE7"/>
+    <mergeCell ref="BF7:BJ7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="M4:M6"/>
     <mergeCell ref="BK7:BO7"/>
     <mergeCell ref="BP7:BT7"/>
     <mergeCell ref="BU7:BY7"/>
@@ -15895,87 +15976,6 @@
     <mergeCell ref="BK4:BK6"/>
     <mergeCell ref="BL4:BL6"/>
     <mergeCell ref="BM4:BM6"/>
-    <mergeCell ref="BN4:BN6"/>
-    <mergeCell ref="BO4:BO6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="AL7:AP7"/>
-    <mergeCell ref="AQ7:AU7"/>
-    <mergeCell ref="AV7:AZ7"/>
-    <mergeCell ref="BA7:BE7"/>
-    <mergeCell ref="BF7:BJ7"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AG7:AK7"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A140:L140"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="U4:U6"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="X4:X6"/>
-    <mergeCell ref="Y4:Y6"/>
-    <mergeCell ref="Z4:Z6"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="AB4:AB6"/>
-    <mergeCell ref="AC4:AC6"/>
-    <mergeCell ref="AD4:AD6"/>
-    <mergeCell ref="AE4:AE6"/>
-    <mergeCell ref="AF4:AF6"/>
-    <mergeCell ref="AG4:AG6"/>
-    <mergeCell ref="AH4:AH6"/>
-    <mergeCell ref="AI4:AI6"/>
-    <mergeCell ref="AJ4:AJ6"/>
-    <mergeCell ref="AK4:AK6"/>
-    <mergeCell ref="AL4:AL6"/>
-    <mergeCell ref="AM4:AM6"/>
-    <mergeCell ref="AN4:AN6"/>
-    <mergeCell ref="AO4:AO6"/>
-    <mergeCell ref="AP4:AP6"/>
-    <mergeCell ref="AQ4:AQ6"/>
-    <mergeCell ref="AR4:AR6"/>
-    <mergeCell ref="AS4:AS6"/>
-    <mergeCell ref="AT4:AT6"/>
-    <mergeCell ref="AU4:AU6"/>
-    <mergeCell ref="AV4:AV6"/>
-    <mergeCell ref="AW4:AW6"/>
-    <mergeCell ref="AX4:AX6"/>
-    <mergeCell ref="AY4:AY6"/>
-    <mergeCell ref="AZ4:AZ6"/>
-    <mergeCell ref="BA4:BA6"/>
-    <mergeCell ref="BG4:BG6"/>
-    <mergeCell ref="BH4:BH6"/>
-    <mergeCell ref="BI4:BI6"/>
-    <mergeCell ref="BJ4:BJ6"/>
-    <mergeCell ref="BB4:BB6"/>
-    <mergeCell ref="BC4:BC6"/>
-    <mergeCell ref="BD4:BD6"/>
-    <mergeCell ref="BE4:BE6"/>
-    <mergeCell ref="BF4:BF6"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E48 E52 E54:E109 E111:E136 E138:E139">
     <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="greaterThan">
@@ -16112,26 +16112,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="62"/>
+      <c r="B1" s="82"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="63"/>
+      <c r="B2" s="83"/>
     </row>
     <row r="3" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="60"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="10">
         <f>COUNTA(B6:B14)</f>
         <v>0</v>
@@ -16203,10 +16203,10 @@
       <c r="B14" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="60"/>
+      <c r="B16" s="80"/>
       <c r="C16" s="10">
         <f>COUNTA(B22:B34)</f>
         <v>0</v>
@@ -16326,10 +16326,10 @@
       <c r="B34" s="13"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="60"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="10">
         <f>COUNTA(B44:B54)</f>
         <v>0</v>
@@ -16449,10 +16449,10 @@
       <c r="B54" s="13"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="60"/>
+      <c r="B56" s="80"/>
       <c r="C56" s="10">
         <f>COUNTA(B58:B67)</f>
         <v>0</v>
@@ -16530,10 +16530,10 @@
       <c r="B67" s="13"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="59" t="s">
+      <c r="A69" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="60"/>
+      <c r="B69" s="80"/>
       <c r="C69" s="10">
         <f>COUNTA(B71:B80)</f>
         <v>0</v>
@@ -16611,10 +16611,10 @@
       <c r="B80" s="13"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="59" t="s">
+      <c r="A82" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="B82" s="60"/>
+      <c r="B82" s="80"/>
       <c r="C82" s="10">
         <f>COUNTA(B84:B93)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Added other APIs end point in config const
</commit_message>
<xml_diff>
--- a/Docs/ShoppingCart WBF.xlsx
+++ b/Docs/ShoppingCart WBF.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VirtusaShoppingCart\Vrt_ShoppingCart\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shiya\Virtusa\Vrt_ShoppingCart\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Effort Summary" sheetId="3" r:id="rId1"/>
-    <sheet name="Assumptions" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Assumptions" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Task_Types">'[1]Effort Summary'!$B$3:$B$25</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="94">
   <si>
     <t>Actual Effort</t>
   </si>
@@ -336,6 +337,18 @@
   </si>
   <si>
     <t>MicroServices Session</t>
+  </si>
+  <si>
+    <t>User create</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Login with credentials</t>
   </si>
 </sst>
 </file>
@@ -875,41 +888,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -930,6 +913,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1680,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="12" ySplit="8" topLeftCell="AC25" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="12" ySplit="8" topLeftCell="BJ126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
@@ -1707,532 +1720,532 @@
       <c r="A1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="72"/>
+      <c r="C1" s="62"/>
       <c r="D1" s="20"/>
       <c r="E1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="20"/>
       <c r="E2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="63">
         <f>SUM(G9:G139)</f>
         <v>470</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M4" s="61">
+      <c r="M4" s="59">
         <v>43983</v>
       </c>
-      <c r="N4" s="61">
+      <c r="N4" s="59">
         <v>43984</v>
       </c>
-      <c r="O4" s="61">
+      <c r="O4" s="59">
         <v>43985</v>
       </c>
-      <c r="P4" s="61">
+      <c r="P4" s="59">
         <v>43986</v>
       </c>
-      <c r="Q4" s="61">
+      <c r="Q4" s="59">
         <v>43987</v>
       </c>
-      <c r="R4" s="61">
+      <c r="R4" s="59">
         <v>43990</v>
       </c>
-      <c r="S4" s="61">
+      <c r="S4" s="59">
         <v>43991</v>
       </c>
-      <c r="T4" s="61">
+      <c r="T4" s="59">
         <v>43992</v>
       </c>
-      <c r="U4" s="61">
+      <c r="U4" s="59">
         <v>43993</v>
       </c>
-      <c r="V4" s="61">
+      <c r="V4" s="59">
         <v>43994</v>
       </c>
-      <c r="W4" s="61">
+      <c r="W4" s="59">
         <v>43997</v>
       </c>
-      <c r="X4" s="61">
+      <c r="X4" s="59">
         <v>43998</v>
       </c>
-      <c r="Y4" s="61">
+      <c r="Y4" s="59">
         <v>43999</v>
       </c>
-      <c r="Z4" s="61">
+      <c r="Z4" s="59">
         <v>44000</v>
       </c>
-      <c r="AA4" s="61">
+      <c r="AA4" s="59">
         <v>44001</v>
       </c>
-      <c r="AB4" s="61">
+      <c r="AB4" s="59">
         <v>44004</v>
       </c>
-      <c r="AC4" s="61">
+      <c r="AC4" s="59">
         <v>44005</v>
       </c>
-      <c r="AD4" s="61">
+      <c r="AD4" s="59">
         <v>44006</v>
       </c>
-      <c r="AE4" s="61">
+      <c r="AE4" s="59">
         <v>44007</v>
       </c>
-      <c r="AF4" s="61">
+      <c r="AF4" s="59">
         <v>44008</v>
       </c>
-      <c r="AG4" s="61">
+      <c r="AG4" s="59">
         <v>44011</v>
       </c>
-      <c r="AH4" s="61">
+      <c r="AH4" s="59">
         <v>44012</v>
       </c>
-      <c r="AI4" s="61">
+      <c r="AI4" s="59">
         <v>44013</v>
       </c>
-      <c r="AJ4" s="61">
+      <c r="AJ4" s="59">
         <v>44014</v>
       </c>
-      <c r="AK4" s="61">
+      <c r="AK4" s="59">
         <v>44015</v>
       </c>
-      <c r="AL4" s="61">
+      <c r="AL4" s="59">
         <v>44018</v>
       </c>
-      <c r="AM4" s="61">
+      <c r="AM4" s="59">
         <v>44019</v>
       </c>
-      <c r="AN4" s="61">
+      <c r="AN4" s="59">
         <v>44020</v>
       </c>
-      <c r="AO4" s="61">
+      <c r="AO4" s="59">
         <v>44021</v>
       </c>
-      <c r="AP4" s="61">
+      <c r="AP4" s="59">
         <v>44022</v>
       </c>
-      <c r="AQ4" s="61">
+      <c r="AQ4" s="59">
         <v>44025</v>
       </c>
-      <c r="AR4" s="61">
+      <c r="AR4" s="59">
         <v>44026</v>
       </c>
-      <c r="AS4" s="61">
+      <c r="AS4" s="59">
         <v>44027</v>
       </c>
-      <c r="AT4" s="61">
+      <c r="AT4" s="59">
         <v>44028</v>
       </c>
-      <c r="AU4" s="61">
+      <c r="AU4" s="59">
         <v>44029</v>
       </c>
-      <c r="AV4" s="61">
+      <c r="AV4" s="59">
         <v>44032</v>
       </c>
-      <c r="AW4" s="61">
+      <c r="AW4" s="59">
         <v>44033</v>
       </c>
-      <c r="AX4" s="61">
+      <c r="AX4" s="59">
         <v>44034</v>
       </c>
-      <c r="AY4" s="61">
+      <c r="AY4" s="59">
         <v>44035</v>
       </c>
-      <c r="AZ4" s="61">
+      <c r="AZ4" s="59">
         <v>44036</v>
       </c>
-      <c r="BA4" s="61">
+      <c r="BA4" s="59">
         <v>44039</v>
       </c>
-      <c r="BB4" s="61">
+      <c r="BB4" s="59">
         <v>44040</v>
       </c>
-      <c r="BC4" s="61">
+      <c r="BC4" s="59">
         <v>44041</v>
       </c>
-      <c r="BD4" s="61">
+      <c r="BD4" s="59">
         <v>44042</v>
       </c>
-      <c r="BE4" s="61">
+      <c r="BE4" s="59">
         <v>44043</v>
       </c>
-      <c r="BF4" s="61">
+      <c r="BF4" s="59">
         <v>44046</v>
       </c>
-      <c r="BG4" s="61">
+      <c r="BG4" s="59">
         <v>44047</v>
       </c>
-      <c r="BH4" s="61">
+      <c r="BH4" s="59">
         <v>44048</v>
       </c>
-      <c r="BI4" s="61">
+      <c r="BI4" s="59">
         <v>44049</v>
       </c>
-      <c r="BJ4" s="61">
+      <c r="BJ4" s="59">
         <v>44050</v>
       </c>
-      <c r="BK4" s="61">
+      <c r="BK4" s="59">
         <v>44053</v>
       </c>
-      <c r="BL4" s="61">
+      <c r="BL4" s="59">
         <v>44054</v>
       </c>
-      <c r="BM4" s="61">
+      <c r="BM4" s="59">
         <v>44055</v>
       </c>
-      <c r="BN4" s="61">
+      <c r="BN4" s="59">
         <v>44056</v>
       </c>
-      <c r="BO4" s="61">
+      <c r="BO4" s="59">
         <v>44057</v>
       </c>
-      <c r="BP4" s="61">
+      <c r="BP4" s="59">
         <v>44060</v>
       </c>
-      <c r="BQ4" s="61">
+      <c r="BQ4" s="59">
         <v>44061</v>
       </c>
-      <c r="BR4" s="61">
+      <c r="BR4" s="59">
         <v>44062</v>
       </c>
-      <c r="BS4" s="61">
+      <c r="BS4" s="59">
         <v>44063</v>
       </c>
-      <c r="BT4" s="61">
+      <c r="BT4" s="59">
         <v>44064</v>
       </c>
-      <c r="BU4" s="61">
+      <c r="BU4" s="59">
         <v>44067</v>
       </c>
-      <c r="BV4" s="61">
+      <c r="BV4" s="59">
         <v>44068</v>
       </c>
-      <c r="BW4" s="61">
+      <c r="BW4" s="59">
         <v>44069</v>
       </c>
-      <c r="BX4" s="61">
+      <c r="BX4" s="59">
         <v>44070</v>
       </c>
-      <c r="BY4" s="61">
+      <c r="BY4" s="59">
         <v>44071</v>
       </c>
     </row>
     <row r="5" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="61"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="61"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="61"/>
-      <c r="Y5" s="61"/>
-      <c r="Z5" s="61"/>
-      <c r="AA5" s="61"/>
-      <c r="AB5" s="61"/>
-      <c r="AC5" s="61"/>
-      <c r="AD5" s="61"/>
-      <c r="AE5" s="61"/>
-      <c r="AF5" s="61"/>
-      <c r="AG5" s="61"/>
-      <c r="AH5" s="61"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="61"/>
-      <c r="AK5" s="61"/>
-      <c r="AL5" s="61"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="61"/>
-      <c r="AP5" s="61"/>
-      <c r="AQ5" s="61"/>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="61"/>
-      <c r="AT5" s="61"/>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="61"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="61"/>
-      <c r="BA5" s="61"/>
-      <c r="BB5" s="61"/>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="61"/>
-      <c r="BE5" s="61"/>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="61"/>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
-      <c r="BK5" s="61"/>
-      <c r="BL5" s="61"/>
-      <c r="BM5" s="61"/>
-      <c r="BN5" s="61"/>
-      <c r="BO5" s="61"/>
-      <c r="BP5" s="61"/>
-      <c r="BQ5" s="61"/>
-      <c r="BR5" s="61"/>
-      <c r="BS5" s="61"/>
-      <c r="BT5" s="61"/>
-      <c r="BU5" s="61"/>
-      <c r="BV5" s="61"/>
-      <c r="BW5" s="61"/>
-      <c r="BX5" s="61"/>
-      <c r="BY5" s="61"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="59"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
+      <c r="AC5" s="59"/>
+      <c r="AD5" s="59"/>
+      <c r="AE5" s="59"/>
+      <c r="AF5" s="59"/>
+      <c r="AG5" s="59"/>
+      <c r="AH5" s="59"/>
+      <c r="AI5" s="59"/>
+      <c r="AJ5" s="59"/>
+      <c r="AK5" s="59"/>
+      <c r="AL5" s="59"/>
+      <c r="AM5" s="59"/>
+      <c r="AN5" s="59"/>
+      <c r="AO5" s="59"/>
+      <c r="AP5" s="59"/>
+      <c r="AQ5" s="59"/>
+      <c r="AR5" s="59"/>
+      <c r="AS5" s="59"/>
+      <c r="AT5" s="59"/>
+      <c r="AU5" s="59"/>
+      <c r="AV5" s="59"/>
+      <c r="AW5" s="59"/>
+      <c r="AX5" s="59"/>
+      <c r="AY5" s="59"/>
+      <c r="AZ5" s="59"/>
+      <c r="BA5" s="59"/>
+      <c r="BB5" s="59"/>
+      <c r="BC5" s="59"/>
+      <c r="BD5" s="59"/>
+      <c r="BE5" s="59"/>
+      <c r="BF5" s="59"/>
+      <c r="BG5" s="59"/>
+      <c r="BH5" s="59"/>
+      <c r="BI5" s="59"/>
+      <c r="BJ5" s="59"/>
+      <c r="BK5" s="59"/>
+      <c r="BL5" s="59"/>
+      <c r="BM5" s="59"/>
+      <c r="BN5" s="59"/>
+      <c r="BO5" s="59"/>
+      <c r="BP5" s="59"/>
+      <c r="BQ5" s="59"/>
+      <c r="BR5" s="59"/>
+      <c r="BS5" s="59"/>
+      <c r="BT5" s="59"/>
+      <c r="BU5" s="59"/>
+      <c r="BV5" s="59"/>
+      <c r="BW5" s="59"/>
+      <c r="BX5" s="59"/>
+      <c r="BY5" s="59"/>
     </row>
     <row r="6" spans="1:77" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="62"/>
-      <c r="X6" s="62"/>
-      <c r="Y6" s="62"/>
-      <c r="Z6" s="62"/>
-      <c r="AA6" s="62"/>
-      <c r="AB6" s="62"/>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="62"/>
-      <c r="AE6" s="62"/>
-      <c r="AF6" s="62"/>
-      <c r="AG6" s="62"/>
-      <c r="AH6" s="62"/>
-      <c r="AI6" s="62"/>
-      <c r="AJ6" s="62"/>
-      <c r="AK6" s="62"/>
-      <c r="AL6" s="62"/>
-      <c r="AM6" s="62"/>
-      <c r="AN6" s="62"/>
-      <c r="AO6" s="62"/>
-      <c r="AP6" s="62"/>
-      <c r="AQ6" s="62"/>
-      <c r="AR6" s="62"/>
-      <c r="AS6" s="62"/>
-      <c r="AT6" s="62"/>
-      <c r="AU6" s="62"/>
-      <c r="AV6" s="62"/>
-      <c r="AW6" s="62"/>
-      <c r="AX6" s="62"/>
-      <c r="AY6" s="62"/>
-      <c r="AZ6" s="62"/>
-      <c r="BA6" s="62"/>
-      <c r="BB6" s="62"/>
-      <c r="BC6" s="62"/>
-      <c r="BD6" s="62"/>
-      <c r="BE6" s="62"/>
-      <c r="BF6" s="62"/>
-      <c r="BG6" s="62"/>
-      <c r="BH6" s="62"/>
-      <c r="BI6" s="62"/>
-      <c r="BJ6" s="62"/>
-      <c r="BK6" s="62"/>
-      <c r="BL6" s="62"/>
-      <c r="BM6" s="62"/>
-      <c r="BN6" s="62"/>
-      <c r="BO6" s="62"/>
-      <c r="BP6" s="62"/>
-      <c r="BQ6" s="62"/>
-      <c r="BR6" s="62"/>
-      <c r="BS6" s="62"/>
-      <c r="BT6" s="62"/>
-      <c r="BU6" s="62"/>
-      <c r="BV6" s="62"/>
-      <c r="BW6" s="62"/>
-      <c r="BX6" s="62"/>
-      <c r="BY6" s="62"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="60"/>
+      <c r="V6" s="60"/>
+      <c r="W6" s="60"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="60"/>
+      <c r="Z6" s="60"/>
+      <c r="AA6" s="60"/>
+      <c r="AB6" s="60"/>
+      <c r="AC6" s="60"/>
+      <c r="AD6" s="60"/>
+      <c r="AE6" s="60"/>
+      <c r="AF6" s="60"/>
+      <c r="AG6" s="60"/>
+      <c r="AH6" s="60"/>
+      <c r="AI6" s="60"/>
+      <c r="AJ6" s="60"/>
+      <c r="AK6" s="60"/>
+      <c r="AL6" s="60"/>
+      <c r="AM6" s="60"/>
+      <c r="AN6" s="60"/>
+      <c r="AO6" s="60"/>
+      <c r="AP6" s="60"/>
+      <c r="AQ6" s="60"/>
+      <c r="AR6" s="60"/>
+      <c r="AS6" s="60"/>
+      <c r="AT6" s="60"/>
+      <c r="AU6" s="60"/>
+      <c r="AV6" s="60"/>
+      <c r="AW6" s="60"/>
+      <c r="AX6" s="60"/>
+      <c r="AY6" s="60"/>
+      <c r="AZ6" s="60"/>
+      <c r="BA6" s="60"/>
+      <c r="BB6" s="60"/>
+      <c r="BC6" s="60"/>
+      <c r="BD6" s="60"/>
+      <c r="BE6" s="60"/>
+      <c r="BF6" s="60"/>
+      <c r="BG6" s="60"/>
+      <c r="BH6" s="60"/>
+      <c r="BI6" s="60"/>
+      <c r="BJ6" s="60"/>
+      <c r="BK6" s="60"/>
+      <c r="BL6" s="60"/>
+      <c r="BM6" s="60"/>
+      <c r="BN6" s="60"/>
+      <c r="BO6" s="60"/>
+      <c r="BP6" s="60"/>
+      <c r="BQ6" s="60"/>
+      <c r="BR6" s="60"/>
+      <c r="BS6" s="60"/>
+      <c r="BT6" s="60"/>
+      <c r="BU6" s="60"/>
+      <c r="BV6" s="60"/>
+      <c r="BW6" s="60"/>
+      <c r="BX6" s="60"/>
+      <c r="BY6" s="60"/>
     </row>
     <row r="7" spans="1:77" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63" t="s">
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="63" t="s">
+      <c r="G7" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="63" t="s">
+      <c r="H7" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="63" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="63" t="s">
+      <c r="I7" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="63" t="s">
+      <c r="K7" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="63" t="s">
+      <c r="L7" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="68" t="s">
+      <c r="M7" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="70"/>
-      <c r="R7" s="68" t="s">
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="70"/>
-      <c r="W7" s="68" t="s">
+      <c r="S7" s="77"/>
+      <c r="T7" s="77"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="78"/>
+      <c r="W7" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="X7" s="69"/>
-      <c r="Y7" s="69"/>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="70"/>
-      <c r="AB7" s="68" t="s">
+      <c r="X7" s="77"/>
+      <c r="Y7" s="77"/>
+      <c r="Z7" s="77"/>
+      <c r="AA7" s="78"/>
+      <c r="AB7" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="AC7" s="69"/>
-      <c r="AD7" s="69"/>
-      <c r="AE7" s="69"/>
-      <c r="AF7" s="70"/>
-      <c r="AG7" s="60" t="s">
+      <c r="AC7" s="77"/>
+      <c r="AD7" s="77"/>
+      <c r="AE7" s="77"/>
+      <c r="AF7" s="78"/>
+      <c r="AG7" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="AH7" s="60"/>
-      <c r="AI7" s="60"/>
-      <c r="AJ7" s="60"/>
-      <c r="AK7" s="60"/>
-      <c r="AL7" s="59" t="s">
+      <c r="AH7" s="75"/>
+      <c r="AI7" s="75"/>
+      <c r="AJ7" s="75"/>
+      <c r="AK7" s="75"/>
+      <c r="AL7" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="AM7" s="59"/>
-      <c r="AN7" s="59"/>
-      <c r="AO7" s="59"/>
-      <c r="AP7" s="59"/>
-      <c r="AQ7" s="59" t="s">
+      <c r="AM7" s="71"/>
+      <c r="AN7" s="71"/>
+      <c r="AO7" s="71"/>
+      <c r="AP7" s="71"/>
+      <c r="AQ7" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="AR7" s="59"/>
-      <c r="AS7" s="59"/>
-      <c r="AT7" s="59"/>
-      <c r="AU7" s="59"/>
-      <c r="AV7" s="59" t="s">
+      <c r="AR7" s="71"/>
+      <c r="AS7" s="71"/>
+      <c r="AT7" s="71"/>
+      <c r="AU7" s="71"/>
+      <c r="AV7" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="AW7" s="59"/>
-      <c r="AX7" s="59"/>
-      <c r="AY7" s="59"/>
-      <c r="AZ7" s="59"/>
-      <c r="BA7" s="65" t="s">
+      <c r="AW7" s="71"/>
+      <c r="AX7" s="71"/>
+      <c r="AY7" s="71"/>
+      <c r="AZ7" s="71"/>
+      <c r="BA7" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="BB7" s="66"/>
-      <c r="BC7" s="66"/>
-      <c r="BD7" s="66"/>
-      <c r="BE7" s="67"/>
-      <c r="BF7" s="60" t="s">
+      <c r="BB7" s="73"/>
+      <c r="BC7" s="73"/>
+      <c r="BD7" s="73"/>
+      <c r="BE7" s="74"/>
+      <c r="BF7" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="BG7" s="60"/>
-      <c r="BH7" s="60"/>
-      <c r="BI7" s="60"/>
-      <c r="BJ7" s="60"/>
-      <c r="BK7" s="59" t="s">
+      <c r="BG7" s="75"/>
+      <c r="BH7" s="75"/>
+      <c r="BI7" s="75"/>
+      <c r="BJ7" s="75"/>
+      <c r="BK7" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="BL7" s="59"/>
-      <c r="BM7" s="59"/>
-      <c r="BN7" s="59"/>
-      <c r="BO7" s="59"/>
-      <c r="BP7" s="59" t="s">
+      <c r="BL7" s="71"/>
+      <c r="BM7" s="71"/>
+      <c r="BN7" s="71"/>
+      <c r="BO7" s="71"/>
+      <c r="BP7" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="BQ7" s="59"/>
-      <c r="BR7" s="59"/>
-      <c r="BS7" s="59"/>
-      <c r="BT7" s="59"/>
-      <c r="BU7" s="60" t="s">
+      <c r="BQ7" s="71"/>
+      <c r="BR7" s="71"/>
+      <c r="BS7" s="71"/>
+      <c r="BT7" s="71"/>
+      <c r="BU7" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="BV7" s="60"/>
-      <c r="BW7" s="60"/>
-      <c r="BX7" s="60"/>
-      <c r="BY7" s="60"/>
+      <c r="BV7" s="75"/>
+      <c r="BW7" s="75"/>
+      <c r="BX7" s="75"/>
+      <c r="BY7" s="75"/>
     </row>
     <row r="8" spans="1:77" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
       <c r="M8" s="24" t="s">
         <v>75</v>
       </c>
@@ -15598,20 +15611,20 @@
       <c r="BY139" s="58"/>
     </row>
     <row r="140" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="A140" s="75" t="s">
+      <c r="A140" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B140" s="76"/>
-      <c r="C140" s="76"/>
-      <c r="D140" s="76"/>
-      <c r="E140" s="76"/>
-      <c r="F140" s="76"/>
-      <c r="G140" s="76"/>
-      <c r="H140" s="76"/>
-      <c r="I140" s="76"/>
-      <c r="J140" s="76"/>
-      <c r="K140" s="76"/>
-      <c r="L140" s="77"/>
+      <c r="B140" s="66"/>
+      <c r="C140" s="66"/>
+      <c r="D140" s="66"/>
+      <c r="E140" s="66"/>
+      <c r="F140" s="66"/>
+      <c r="G140" s="66"/>
+      <c r="H140" s="66"/>
+      <c r="I140" s="66"/>
+      <c r="J140" s="66"/>
+      <c r="K140" s="66"/>
+      <c r="L140" s="67"/>
       <c r="M140" s="31">
         <f>SUM(M10:M139)</f>
         <v>0</v>
@@ -15879,55 +15892,38 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="BG4:BG6"/>
-    <mergeCell ref="BH4:BH6"/>
-    <mergeCell ref="BI4:BI6"/>
-    <mergeCell ref="BJ4:BJ6"/>
-    <mergeCell ref="BB4:BB6"/>
-    <mergeCell ref="BC4:BC6"/>
-    <mergeCell ref="BD4:BD6"/>
-    <mergeCell ref="BE4:BE6"/>
-    <mergeCell ref="BF4:BF6"/>
-    <mergeCell ref="AW4:AW6"/>
-    <mergeCell ref="AX4:AX6"/>
-    <mergeCell ref="AY4:AY6"/>
-    <mergeCell ref="AZ4:AZ6"/>
-    <mergeCell ref="BA4:BA6"/>
-    <mergeCell ref="AR4:AR6"/>
-    <mergeCell ref="AS4:AS6"/>
-    <mergeCell ref="AT4:AT6"/>
-    <mergeCell ref="AU4:AU6"/>
-    <mergeCell ref="AV4:AV6"/>
-    <mergeCell ref="AM4:AM6"/>
-    <mergeCell ref="AN4:AN6"/>
-    <mergeCell ref="AO4:AO6"/>
-    <mergeCell ref="AP4:AP6"/>
-    <mergeCell ref="AQ4:AQ6"/>
-    <mergeCell ref="AH4:AH6"/>
-    <mergeCell ref="AI4:AI6"/>
-    <mergeCell ref="AJ4:AJ6"/>
-    <mergeCell ref="AK4:AK6"/>
-    <mergeCell ref="AL4:AL6"/>
-    <mergeCell ref="AC4:AC6"/>
-    <mergeCell ref="AD4:AD6"/>
-    <mergeCell ref="AE4:AE6"/>
-    <mergeCell ref="AF4:AF6"/>
-    <mergeCell ref="AG4:AG6"/>
-    <mergeCell ref="X4:X6"/>
-    <mergeCell ref="Y4:Y6"/>
-    <mergeCell ref="Z4:Z6"/>
-    <mergeCell ref="AA4:AA6"/>
-    <mergeCell ref="AB4:AB6"/>
-    <mergeCell ref="S4:S6"/>
-    <mergeCell ref="T4:T6"/>
-    <mergeCell ref="U4:U6"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="O4:O6"/>
-    <mergeCell ref="P4:P6"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="BK7:BO7"/>
+    <mergeCell ref="BP7:BT7"/>
+    <mergeCell ref="BU7:BY7"/>
+    <mergeCell ref="BU4:BU6"/>
+    <mergeCell ref="BV4:BV6"/>
+    <mergeCell ref="BW4:BW6"/>
+    <mergeCell ref="BX4:BX6"/>
+    <mergeCell ref="BY4:BY6"/>
+    <mergeCell ref="BP4:BP6"/>
+    <mergeCell ref="BQ4:BQ6"/>
+    <mergeCell ref="BR4:BR6"/>
+    <mergeCell ref="BS4:BS6"/>
+    <mergeCell ref="BT4:BT6"/>
+    <mergeCell ref="BK4:BK6"/>
+    <mergeCell ref="BL4:BL6"/>
+    <mergeCell ref="BM4:BM6"/>
+    <mergeCell ref="BN4:BN6"/>
+    <mergeCell ref="BO4:BO6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="AL7:AP7"/>
+    <mergeCell ref="AQ7:AU7"/>
+    <mergeCell ref="AV7:AZ7"/>
+    <mergeCell ref="BA7:BE7"/>
+    <mergeCell ref="BF7:BJ7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AG7:AK7"/>
+    <mergeCell ref="M4:M6"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="A140:L140"/>
@@ -15944,38 +15940,55 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="BN4:BN6"/>
-    <mergeCell ref="BO4:BO6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="AL7:AP7"/>
-    <mergeCell ref="AQ7:AU7"/>
-    <mergeCell ref="AV7:AZ7"/>
-    <mergeCell ref="BA7:BE7"/>
-    <mergeCell ref="BF7:BJ7"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AG7:AK7"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="BK7:BO7"/>
-    <mergeCell ref="BP7:BT7"/>
-    <mergeCell ref="BU7:BY7"/>
-    <mergeCell ref="BU4:BU6"/>
-    <mergeCell ref="BV4:BV6"/>
-    <mergeCell ref="BW4:BW6"/>
-    <mergeCell ref="BX4:BX6"/>
-    <mergeCell ref="BY4:BY6"/>
-    <mergeCell ref="BP4:BP6"/>
-    <mergeCell ref="BQ4:BQ6"/>
-    <mergeCell ref="BR4:BR6"/>
-    <mergeCell ref="BS4:BS6"/>
-    <mergeCell ref="BT4:BT6"/>
-    <mergeCell ref="BK4:BK6"/>
-    <mergeCell ref="BL4:BL6"/>
-    <mergeCell ref="BM4:BM6"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="O4:O6"/>
+    <mergeCell ref="P4:P6"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:S6"/>
+    <mergeCell ref="T4:T6"/>
+    <mergeCell ref="U4:U6"/>
+    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="X4:X6"/>
+    <mergeCell ref="Y4:Y6"/>
+    <mergeCell ref="Z4:Z6"/>
+    <mergeCell ref="AA4:AA6"/>
+    <mergeCell ref="AB4:AB6"/>
+    <mergeCell ref="AC4:AC6"/>
+    <mergeCell ref="AD4:AD6"/>
+    <mergeCell ref="AE4:AE6"/>
+    <mergeCell ref="AF4:AF6"/>
+    <mergeCell ref="AG4:AG6"/>
+    <mergeCell ref="AH4:AH6"/>
+    <mergeCell ref="AI4:AI6"/>
+    <mergeCell ref="AJ4:AJ6"/>
+    <mergeCell ref="AK4:AK6"/>
+    <mergeCell ref="AL4:AL6"/>
+    <mergeCell ref="AM4:AM6"/>
+    <mergeCell ref="AN4:AN6"/>
+    <mergeCell ref="AO4:AO6"/>
+    <mergeCell ref="AP4:AP6"/>
+    <mergeCell ref="AQ4:AQ6"/>
+    <mergeCell ref="AR4:AR6"/>
+    <mergeCell ref="AS4:AS6"/>
+    <mergeCell ref="AT4:AT6"/>
+    <mergeCell ref="AU4:AU6"/>
+    <mergeCell ref="AV4:AV6"/>
+    <mergeCell ref="AW4:AW6"/>
+    <mergeCell ref="AX4:AX6"/>
+    <mergeCell ref="AY4:AY6"/>
+    <mergeCell ref="AZ4:AZ6"/>
+    <mergeCell ref="BA4:BA6"/>
+    <mergeCell ref="BG4:BG6"/>
+    <mergeCell ref="BH4:BH6"/>
+    <mergeCell ref="BI4:BI6"/>
+    <mergeCell ref="BJ4:BJ6"/>
+    <mergeCell ref="BB4:BB6"/>
+    <mergeCell ref="BC4:BC6"/>
+    <mergeCell ref="BD4:BD6"/>
+    <mergeCell ref="BE4:BE6"/>
+    <mergeCell ref="BF4:BF6"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E48 E52 E54:E109 E111:E136 E138:E139">
     <cfRule type="cellIs" dxfId="24" priority="25" stopIfTrue="1" operator="greaterThan">
@@ -16097,6 +16110,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView topLeftCell="A77" workbookViewId="0">

</xml_diff>